<commit_message>
Add 16 09 @SvyTo
</commit_message>
<xml_diff>
--- a/RPL_V2/xlsx/Матч Тура 24-25.xlsx
+++ b/RPL_V2/xlsx/Матч Тура 24-25.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="mt_rostov_cska" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,12 @@
     <sheet name="mt_spartak_dinamo" sheetId="9" r:id="rId9"/>
     <sheet name="mt_krasnodar_zenit" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4339" uniqueCount="1093">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4655" uniqueCount="1147">
   <si>
     <t>type</t>
   </si>
@@ -3282,9 +3282,6 @@
     <t>На каком месте находится Динамо Москва после шести туров?</t>
   </si>
   <si>
-    <t>Кого обыграл Спартак в прошлом туре?</t>
-  </si>
-  <si>
     <t>На каком месте находится Спартак после шести туров?</t>
   </si>
   <si>
@@ -3307,6 +3304,171 @@
   </si>
   <si>
     <t>Мексика</t>
+  </si>
+  <si>
+    <t>sm_abena</t>
+  </si>
+  <si>
+    <t>sm_markinios</t>
+  </si>
+  <si>
+    <t>Амкал</t>
+  </si>
+  <si>
+    <t>Какой по счету сейчас тур?</t>
+  </si>
+  <si>
+    <t>Кто забил победный для Динамо Москва мяч в прошлом туре?</t>
+  </si>
+  <si>
+    <t>Как звучит полное имя игрока Динамо Москва - Муми Нгамалё?</t>
+  </si>
+  <si>
+    <t>С каким счетом завершилась для Спартака встреча с махачкалинским Динаом в прошлом туре?</t>
+  </si>
+  <si>
+    <t>1:1</t>
+  </si>
+  <si>
+    <t>0:0</t>
+  </si>
+  <si>
+    <t>На 5 месте</t>
+  </si>
+  <si>
+    <t>На 4 месте</t>
+  </si>
+  <si>
+    <t>На 3 месте</t>
+  </si>
+  <si>
+    <t>На 2 месте</t>
+  </si>
+  <si>
+    <t>на 6 месте</t>
+  </si>
+  <si>
+    <t>На 7 месте</t>
+  </si>
+  <si>
+    <t>На 1 месте</t>
+  </si>
+  <si>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/mt_spartak_dinamo.jpg</t>
+  </si>
+  <si>
+    <t>Гватемала</t>
+  </si>
+  <si>
+    <t>Гваделупа</t>
+  </si>
+  <si>
+    <t>Гренада</t>
+  </si>
+  <si>
+    <t>Победой какой команды завершился последний матч между Спартаком и Динамо?</t>
+  </si>
+  <si>
+    <t>Канада</t>
+  </si>
+  <si>
+    <t>Новая Зеландия</t>
+  </si>
+  <si>
+    <t>Австралия</t>
+  </si>
+  <si>
+    <t>Эквадор</t>
+  </si>
+  <si>
+    <t>Кто этот знаменитый футболист, игрок Динамо в прошлом?</t>
+  </si>
+  <si>
+    <t>Кристиан Нобоа</t>
+  </si>
+  <si>
+    <t>Кто является лучшим бомбардиром Спартака в этом сезоне РПЛ?</t>
+  </si>
+  <si>
+    <t>Абена Миенти</t>
+  </si>
+  <si>
+    <t>Даниил Хлусевич</t>
+  </si>
+  <si>
+    <t>Олег Рябчук</t>
+  </si>
+  <si>
+    <t>Маркиньос</t>
+  </si>
+  <si>
+    <t>dm_makarov</t>
+  </si>
+  <si>
+    <t>dm_mauhub</t>
+  </si>
+  <si>
+    <t>21-летний (05.06.2003) марокканский нападающий. Перешёл в Динамо Москва летом 2024 из Раджа Касабланка</t>
+  </si>
+  <si>
+    <t>Эль-Мехди Маухуб</t>
+  </si>
+  <si>
+    <t>Слован Братислава</t>
+  </si>
+  <si>
+    <t>Спартак Трнава</t>
+  </si>
+  <si>
+    <t>Графсхап</t>
+  </si>
+  <si>
+    <t>Утрехт</t>
+  </si>
+  <si>
+    <t>Брага</t>
+  </si>
+  <si>
+    <t>Шанхай Шэньхуа</t>
+  </si>
+  <si>
+    <t>Кассио</t>
+  </si>
+  <si>
+    <t>Матеус Перейра</t>
+  </si>
+  <si>
+    <t>Уоллас</t>
+  </si>
+  <si>
+    <t>Рафаэль Борре</t>
+  </si>
+  <si>
+    <t>Тиаго Майя</t>
+  </si>
+  <si>
+    <t>8 тур</t>
+  </si>
+  <si>
+    <t>7 тур</t>
+  </si>
+  <si>
+    <t>6 тур</t>
+  </si>
+  <si>
+    <t>9 тур</t>
+  </si>
+  <si>
+    <t>10 тур</t>
+  </si>
+  <si>
+    <t>11 тур</t>
+  </si>
+  <si>
+    <t>num_9</t>
+  </si>
+  <si>
+    <t>num_11</t>
   </si>
 </sst>
 </file>
@@ -3337,18 +3499,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -3382,7 +3538,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3396,8 +3552,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -11353,7 +11516,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B9:B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -14572,7 +14737,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16306,7 +16473,7 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:B26"/>
+      <selection activeCell="B32" sqref="B9:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18039,10 +18206,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q32"/>
+  <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q36" sqref="A2:Q36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18051,10 +18218,10 @@
     <col min="2" max="2" width="124.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
     <col min="11" max="11" width="26" customWidth="1"/>
@@ -18063,7 +18230,7 @@
     <col min="14" max="14" width="11" customWidth="1"/>
     <col min="15" max="15" width="22" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
-    <col min="17" max="17" width="18" customWidth="1"/>
+    <col min="17" max="17" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -18119,189 +18286,423 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C2" s="4" t="s">
+        <v>1092</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>1120</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>745</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>1122</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="C3" s="4" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>1093</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>744</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>743</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>747</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>753</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
+      <c r="C4" s="4" t="s">
+        <v>740</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>741</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>740</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>742</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>743</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>744</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>745</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>746</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>747</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="4">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
+      <c r="C5" s="4" t="s">
+        <v>826</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>826</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>744</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>745</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>1122</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>753</v>
+      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>2</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="4">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
+      <c r="C6" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>2</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="4">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
+      <c r="C7" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>2</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="4">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
+      <c r="C8" s="4" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>1124</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>565</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>2</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="A9" s="4">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
+      <c r="C9" s="4" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>1126</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>1127</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -18416,7 +18817,9 @@
       <c r="B12" s="2" t="s">
         <v>1051</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="4" t="s">
+        <v>1092</v>
+      </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
@@ -18428,23 +18831,33 @@
       <c r="H12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="2"/>
+      <c r="I12" s="2" t="s">
+        <v>1128</v>
+      </c>
       <c r="J12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="2"/>
+      <c r="K12" s="2" t="s">
+        <v>1129</v>
+      </c>
       <c r="L12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M12" s="2"/>
+      <c r="M12" s="2" t="s">
+        <v>1130</v>
+      </c>
       <c r="N12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O12" s="2"/>
+      <c r="O12" s="2" t="s">
+        <v>1131</v>
+      </c>
       <c r="P12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Q12" s="2"/>
+      <c r="Q12" s="2" t="s">
+        <v>1132</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -18453,7 +18866,9 @@
       <c r="B13" s="2" t="s">
         <v>1052</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="4" t="s">
+        <v>1093</v>
+      </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -18500,7 +18915,9 @@
       <c r="B14" s="2" t="s">
         <v>1055</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="4" t="s">
+        <v>826</v>
+      </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -18512,28 +18929,44 @@
       <c r="H14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I14" s="2"/>
+      <c r="I14" s="2">
+        <v>30</v>
+      </c>
       <c r="J14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K14" s="2"/>
+      <c r="K14" s="2">
+        <v>27</v>
+      </c>
       <c r="L14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M14" s="2"/>
+      <c r="M14" s="2">
+        <v>21</v>
+      </c>
       <c r="N14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O14" s="2"/>
+      <c r="O14" s="2">
+        <v>19</v>
+      </c>
       <c r="P14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Q14" s="2"/>
+      <c r="Q14" s="2">
+        <v>35</v>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
       <c r="B15" s="2" t="s">
         <v>1064</v>
       </c>
+      <c r="C15" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
       <c r="F15" s="2" t="s">
         <v>20</v>
       </c>
@@ -18543,23 +18976,42 @@
       <c r="H15" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="I15" s="4" t="s">
+        <v>336</v>
+      </c>
       <c r="J15" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="K15" s="4" t="s">
+        <v>1094</v>
+      </c>
       <c r="L15" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="M15" s="4" t="s">
+        <v>838</v>
+      </c>
       <c r="N15" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="O15" s="4" t="s">
+        <v>287</v>
+      </c>
       <c r="P15" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="Q15" s="4" t="s">
+        <v>1133</v>
+      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
       <c r="B16" s="2" t="s">
         <v>1066</v>
       </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
       <c r="F16" s="2" t="s">
         <v>20</v>
       </c>
@@ -18569,23 +19021,42 @@
       <c r="H16" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="I16" s="4" t="s">
+        <v>1134</v>
+      </c>
       <c r="J16" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="K16" s="4" t="s">
+        <v>1135</v>
+      </c>
       <c r="L16" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="M16" s="4" t="s">
+        <v>1136</v>
+      </c>
       <c r="N16" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="O16" s="4" t="s">
+        <v>1137</v>
+      </c>
       <c r="P16" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="Q16" s="4" t="s">
+        <v>1138</v>
+      </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
       <c r="B17" s="2" t="s">
         <v>1067</v>
       </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
       <c r="F17" s="2" t="s">
         <v>20</v>
       </c>
@@ -18595,23 +19066,44 @@
       <c r="H17" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="I17" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="J17" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="K17" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="L17" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="M17" s="2" t="s">
+        <v>352</v>
+      </c>
       <c r="N17" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="O17" s="2" t="s">
+        <v>425</v>
+      </c>
       <c r="P17" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="Q17" s="2" t="s">
+        <v>1094</v>
+      </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
       <c r="B18" s="2" t="s">
         <v>1069</v>
       </c>
+      <c r="C18" s="7" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="7"/>
       <c r="F18" s="2" t="s">
         <v>20</v>
       </c>
@@ -18621,48 +19113,74 @@
       <c r="H18" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="I18" s="4"/>
       <c r="J18" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="K18" s="4"/>
       <c r="L18" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="M18" s="4"/>
       <c r="N18" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="O18" s="4"/>
       <c r="P18" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="Q18" s="4"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
       <c r="B19" s="2" t="s">
         <v>1069</v>
       </c>
+      <c r="C19" s="7" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="7" t="s">
+        <v>1108</v>
+      </c>
       <c r="F19" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="G19" s="4"/>
       <c r="H19" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="I19" s="4"/>
       <c r="J19" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="K19" s="4"/>
       <c r="L19" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="M19" s="4"/>
       <c r="N19" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="O19" s="4"/>
       <c r="P19" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="Q19" s="4"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
       <c r="B20" s="2" t="s">
         <v>1071</v>
       </c>
-      <c r="D20" t="s">
+      <c r="C20" s="7" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>1074</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>1108</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>20</v>
@@ -18673,23 +19191,34 @@
       <c r="H20" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="I20" s="4"/>
       <c r="J20" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="K20" s="4"/>
       <c r="L20" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="M20" s="4"/>
       <c r="N20" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="O20" s="4"/>
       <c r="P20" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="Q20" s="4"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
       <c r="B21" s="2" t="s">
         <v>1073</v>
       </c>
+      <c r="C21" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
       <c r="F21" s="2" t="s">
         <v>20</v>
       </c>
@@ -18723,77 +19252,437 @@
       <c r="P21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="Q21" s="4" t="s">
         <v>1079</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
       <c r="B22" s="2" t="s">
         <v>1081</v>
       </c>
+      <c r="C22" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="O22" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="P22" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q22" s="4" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
       <c r="B23" s="2" t="s">
         <v>579</v>
       </c>
+      <c r="C23" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4" t="s">
+        <v>729</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>729</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>730</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>900</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>1030</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="O23" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="P23" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="Q23" s="4" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
       <c r="B24" s="2" t="s">
-        <v>1084</v>
+        <v>1098</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>1099</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>583</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>1100</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>581</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O24" s="6" t="s">
+        <v>582</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q24" s="6" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
       <c r="B25" s="2" t="s">
         <v>1082</v>
       </c>
+      <c r="C25" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="M25" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="N25" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="O25" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="P25" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q25" s="4" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
       <c r="B26" s="2" t="s">
-        <v>1085</v>
+        <v>1084</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>1101</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>1102</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>1103</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>1104</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="O26" s="4" t="s">
+        <v>1105</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q26" s="4" t="s">
+        <v>1106</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
       <c r="B27" s="2" t="s">
         <v>1083</v>
       </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>1102</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>1103</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>1104</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="M27" s="4" t="s">
+        <v>1105</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="O27" s="4" t="s">
+        <v>1101</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="Q27" s="4" t="s">
+        <v>1107</v>
+      </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
       <c r="B28" s="2" t="s">
+        <v>1085</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" s="4" t="s">
         <v>1086</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I28" s="4" t="s">
         <v>1087</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>1087</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M28" s="4" t="s">
+        <v>1087</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O28" s="4" t="s">
+        <v>1087</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q28" s="4" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="2" t="s">
         <v>1088</v>
       </c>
-      <c r="K28" t="s">
-        <v>1088</v>
-      </c>
-      <c r="M28" t="s">
-        <v>1088</v>
-      </c>
-      <c r="O28" t="s">
-        <v>1088</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>1088</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="4" t="s">
+        <v>752</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" s="4" t="s">
         <v>1089</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>1109</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>1091</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M29" s="4" t="s">
+        <v>1110</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O29" s="4" t="s">
+        <v>829</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q29" s="4" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="2" t="s">
         <v>1090</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G30" s="4" t="s">
         <v>1091</v>
       </c>
-      <c r="G30" t="s">
-        <v>1092</v>
+      <c r="H30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>1113</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>829</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>1114</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O30" s="4" t="s">
+        <v>1115</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q30" s="4" t="s">
+        <v>1116</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -18852,7 +19741,7 @@
         <v>1</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>359</v>
+        <v>1097</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>360</v>
@@ -18900,8 +19789,211 @@
         <v>367</v>
       </c>
     </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="2" t="s">
+        <v>1095</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>1139</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>1140</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>1141</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>1145</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>1142</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>1146</v>
+      </c>
+      <c r="O33" s="4" t="s">
+        <v>1143</v>
+      </c>
+      <c r="P33" s="2" t="s">
+        <v>1146</v>
+      </c>
+      <c r="Q33" s="4" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="2" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4" t="s">
+        <v>1124</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>1125</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>1127</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="L34" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="M34" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="N34" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="O34" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="P34" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="Q34" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="2" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M35" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O35" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="P35" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q35" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="2" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I36" s="4"/>
+      <c r="J36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K36" s="4"/>
+      <c r="L36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M36" s="4"/>
+      <c r="N36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O36" s="4"/>
+      <c r="P36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q36" s="4"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E37" t="s">
+        <v>752</v>
+      </c>
+      <c r="F37" t="s">
+        <v>752</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>745</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C18" r:id="rId1"/>
+    <hyperlink ref="C19" r:id="rId2"/>
+    <hyperlink ref="C20" r:id="rId3"/>
+    <hyperlink ref="E20" r:id="rId4"/>
+    <hyperlink ref="E19" r:id="rId5"/>
+    <hyperlink ref="C35" r:id="rId6"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add 16 09 + mt @SvyTo
</commit_message>
<xml_diff>
--- a/RPL_V2/xlsx/Матч Тура 24-25.xlsx
+++ b/RPL_V2/xlsx/Матч Тура 24-25.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4751" uniqueCount="1180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4757" uniqueCount="1186">
   <si>
     <t>type</t>
   </si>
@@ -3330,12 +3330,6 @@
     <t>Соперничество футбольных клубов «Динамо» и «Спартак» — старейшее из российских и московских дерби, берущее начало с первого матча «Красная Пресня» — «Динамо» 17 июня 1923 года в чемпионате Москвы.</t>
   </si>
   <si>
-    <t>https://amaranth64.github.io/RPL_V2/matchday/mt_spartak_dinamo.jpg</t>
-  </si>
-  <si>
-    <t>17 июня 1923 года</t>
-  </si>
-  <si>
     <t>17 августа 1944</t>
   </si>
   <si>
@@ -3375,9 +3369,6 @@
     <t>С кем сыграет Спартак в следующем туре?</t>
   </si>
   <si>
-    <t>С каким счетом завершилась для Спартака встреча с махачкалинским Динаом в прошлом туре?</t>
-  </si>
-  <si>
     <t>1:1</t>
   </si>
   <si>
@@ -3568,6 +3559,33 @@
   </si>
   <si>
     <t>Уилсон Исидор</t>
+  </si>
+  <si>
+    <t>logo_dinamo_mah</t>
+  </si>
+  <si>
+    <t>32 года</t>
+  </si>
+  <si>
+    <t>30 лет</t>
+  </si>
+  <si>
+    <t>27 лет</t>
+  </si>
+  <si>
+    <t>21 год</t>
+  </si>
+  <si>
+    <t>19 лет</t>
+  </si>
+  <si>
+    <t>35 лет</t>
+  </si>
+  <si>
+    <t>С каким счетом завершилась для Спартака встреча с махачкалинским Динамо в прошлом туре?</t>
+  </si>
+  <si>
+    <t>17 июня 1923</t>
   </si>
 </sst>
 </file>
@@ -5953,7 +5971,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>1172</v>
+        <v>1169</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -5962,7 +5980,7 @@
         <v>20</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>1173</v>
+        <v>1170</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>20</v>
@@ -5990,7 +6008,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>1174</v>
+        <v>1171</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -5999,7 +6017,7 @@
         <v>20</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>1175</v>
+        <v>1172</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>20</v>
@@ -6027,7 +6045,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>1176</v>
+        <v>1173</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -6036,7 +6054,7 @@
         <v>20</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>1177</v>
+        <v>1174</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>20</v>
@@ -6064,7 +6082,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>1178</v>
+        <v>1175</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -6073,7 +6091,7 @@
         <v>20</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>1179</v>
+        <v>1176</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>20</v>
@@ -6105,7 +6123,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="E1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9853,7 +9871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="E1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11752,7 +11770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="E1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13384,7 +13402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="D1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16704,7 +16722,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18438,8 +18458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18449,7 +18469,7 @@
     <col min="3" max="3" width="75" customWidth="1"/>
     <col min="4" max="4" width="198" customWidth="1"/>
     <col min="5" max="5" width="75" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="24" customWidth="1"/>
@@ -19161,38 +19181,38 @@
       <c r="F14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="2">
-        <v>32</v>
+      <c r="G14" s="2" t="s">
+        <v>1178</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I14" s="2">
-        <v>30</v>
+      <c r="I14" s="2" t="s">
+        <v>1179</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K14" s="2">
-        <v>27</v>
+      <c r="K14" s="2" t="s">
+        <v>1180</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M14" s="2">
-        <v>21</v>
+      <c r="M14" s="2" t="s">
+        <v>1181</v>
       </c>
       <c r="N14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O14" s="2">
-        <v>19</v>
+      <c r="O14" s="2" t="s">
+        <v>1182</v>
       </c>
       <c r="P14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Q14" s="2">
-        <v>35</v>
+      <c r="Q14" s="2" t="s">
+        <v>1183</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -19464,43 +19484,43 @@
         <v>1099</v>
       </c>
       <c r="E20" s="3" t="s">
+        <v>1086</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>1185</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="2" t="s">
         <v>1100</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G20" s="2" t="s">
+      <c r="J20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K20" s="2" t="s">
         <v>1101</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I20" s="2" t="s">
+      <c r="L20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M20" s="2" t="s">
         <v>1102</v>
       </c>
-      <c r="J20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K20" s="2" t="s">
+      <c r="N20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O20" s="2" t="s">
         <v>1103</v>
       </c>
-      <c r="L20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M20" s="2" t="s">
+      <c r="P20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q20" s="2" t="s">
         <v>1104</v>
-      </c>
-      <c r="N20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O20" s="2" t="s">
-        <v>1105</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q20" s="2" t="s">
-        <v>1106</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -19508,7 +19528,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>136</v>
@@ -19521,37 +19541,37 @@
         <v>20</v>
       </c>
       <c r="G21" s="2" t="s">
+        <v>1106</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>1107</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K21" s="2" t="s">
         <v>1108</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I21" s="2" t="s">
+      <c r="L21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M21" s="2" t="s">
         <v>1109</v>
       </c>
-      <c r="J21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K21" s="2" t="s">
+      <c r="N21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O21" s="2" t="s">
         <v>1110</v>
       </c>
-      <c r="L21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M21" s="2" t="s">
+      <c r="P21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q21" s="2" t="s">
         <v>1111</v>
-      </c>
-      <c r="N21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O21" s="2" t="s">
-        <v>1112</v>
-      </c>
-      <c r="P21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q21" s="2" t="s">
-        <v>1113</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -19559,7 +19579,7 @@
         <v>2</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>136</v>
@@ -19620,7 +19640,7 @@
         <v>729</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>729</v>
+        <v>1177</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>730</v>
@@ -19661,7 +19681,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>1115</v>
+        <v>1184</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>136</v>
@@ -19674,7 +19694,7 @@
         <v>20</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>1116</v>
+        <v>1113</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>20</v>
@@ -19686,7 +19706,7 @@
         <v>20</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>1117</v>
+        <v>1114</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>20</v>
@@ -19712,7 +19732,7 @@
         <v>2</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>132</v>
@@ -19763,7 +19783,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>1119</v>
+        <v>1116</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>20</v>
@@ -19776,37 +19796,37 @@
         <v>183</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>1120</v>
+        <v>1117</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>181</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>1121</v>
+        <v>1118</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>179</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>1122</v>
+        <v>1119</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>177</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>1123</v>
+        <v>1120</v>
       </c>
       <c r="N26" s="2" t="s">
         <v>185</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>1124</v>
+        <v>1121</v>
       </c>
       <c r="P26" s="2" t="s">
         <v>187</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -19814,7 +19834,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>1126</v>
+        <v>1123</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>20</v>
@@ -19827,37 +19847,37 @@
         <v>181</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>1121</v>
+        <v>1118</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>179</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>1122</v>
+        <v>1119</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>177</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>1123</v>
+        <v>1120</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>185</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>1124</v>
+        <v>1121</v>
       </c>
       <c r="N27" s="2" t="s">
         <v>183</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>1120</v>
+        <v>1117</v>
       </c>
       <c r="P27" s="2" t="s">
         <v>490</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>1127</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -19865,7 +19885,7 @@
         <v>6</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>1128</v>
+        <v>1125</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>825</v>
@@ -19878,37 +19898,37 @@
         <v>20</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>1129</v>
+        <v>1126</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>20</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>1130</v>
+        <v>1127</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>1130</v>
+        <v>1127</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>20</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>1130</v>
+        <v>1127</v>
       </c>
       <c r="N28" s="2" t="s">
         <v>20</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>1130</v>
+        <v>1127</v>
       </c>
       <c r="P28" s="2" t="s">
         <v>20</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>1130</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -19916,7 +19936,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>1131</v>
+        <v>1128</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>752</v>
@@ -19929,25 +19949,25 @@
         <v>20</v>
       </c>
       <c r="G29" s="2" t="s">
+        <v>1129</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>1131</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M29" s="2" t="s">
         <v>1132</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>1133</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>1134</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>1135</v>
       </c>
       <c r="N29" s="2" t="s">
         <v>20</v>
@@ -19959,7 +19979,7 @@
         <v>20</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>1136</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -19967,7 +19987,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>1137</v>
+        <v>1134</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>236</v>
@@ -19980,13 +20000,13 @@
         <v>20</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>1134</v>
+        <v>1131</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>20</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>1138</v>
+        <v>1135</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>20</v>
@@ -19998,19 +20018,19 @@
         <v>20</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>1139</v>
+        <v>1136</v>
       </c>
       <c r="N30" s="2" t="s">
         <v>20</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>1140</v>
+        <v>1137</v>
       </c>
       <c r="P30" s="2" t="s">
         <v>20</v>
       </c>
       <c r="Q30" s="2" t="s">
-        <v>1141</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -20069,7 +20089,7 @@
         <v>1</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>1142</v>
+        <v>1139</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>360</v>
@@ -20122,7 +20142,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>1143</v>
+        <v>1140</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>20</v>
@@ -20135,37 +20155,37 @@
         <v>212</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>1144</v>
+        <v>1141</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>187</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>185</v>
       </c>
       <c r="K33" s="2" t="s">
+        <v>1143</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>1144</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>1145</v>
+      </c>
+      <c r="N33" s="2" t="s">
         <v>1146</v>
       </c>
-      <c r="L33" s="2" t="s">
+      <c r="O33" s="2" t="s">
         <v>1147</v>
       </c>
-      <c r="M33" s="2" t="s">
+      <c r="P33" s="2" t="s">
+        <v>1146</v>
+      </c>
+      <c r="Q33" s="2" t="s">
         <v>1148</v>
-      </c>
-      <c r="N33" s="2" t="s">
-        <v>1149</v>
-      </c>
-      <c r="O33" s="2" t="s">
-        <v>1150</v>
-      </c>
-      <c r="P33" s="2" t="s">
-        <v>1149</v>
-      </c>
-      <c r="Q33" s="2" t="s">
-        <v>1151</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
@@ -20173,7 +20193,7 @@
         <v>2</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>1152</v>
+        <v>1149</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>132</v>
@@ -20224,7 +20244,7 @@
         <v>6</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>1153</v>
+        <v>1150</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>1086</v>
@@ -20275,32 +20295,32 @@
         <v>1</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="3" t="s">
+        <v>1152</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>1153</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>1154</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K36" s="2" t="s">
         <v>1155</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>1156</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>1157</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>1158</v>
       </c>
       <c r="L36" s="2" t="s">
         <v>20</v>
@@ -20312,13 +20332,13 @@
         <v>20</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>1159</v>
+        <v>1156</v>
       </c>
       <c r="P36" s="2" t="s">
         <v>20</v>
       </c>
       <c r="Q36" s="2" t="s">
-        <v>1160</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
@@ -20326,7 +20346,7 @@
         <v>2</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>1161</v>
+        <v>1158</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>136</v>
@@ -20354,16 +20374,16 @@
         <v>746</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>1162</v>
+        <v>1159</v>
       </c>
       <c r="M37" s="2" t="s">
         <v>406</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>1163</v>
+        <v>1160</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>1164</v>
+        <v>1161</v>
       </c>
       <c r="P37" s="2" t="s">
         <v>826</v>
@@ -20390,7 +20410,7 @@
         <v>20</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>1165</v>
+        <v>1162</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>20</v>
@@ -20402,13 +20422,13 @@
         <v>20</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>1166</v>
+        <v>1163</v>
       </c>
       <c r="L38" s="2" t="s">
         <v>20</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>1167</v>
+        <v>1164</v>
       </c>
       <c r="N38" s="2" t="s">
         <v>20</v>
@@ -20453,25 +20473,25 @@
         <v>20</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>1168</v>
+        <v>1165</v>
       </c>
       <c r="L39" s="2" t="s">
         <v>20</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>1169</v>
+        <v>1166</v>
       </c>
       <c r="N39" s="2" t="s">
         <v>20</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>1170</v>
+        <v>1167</v>
       </c>
       <c r="P39" s="2" t="s">
         <v>20</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>1156</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -20510,7 +20530,7 @@
         <v>20</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>1171</v>
+        <v>1168</v>
       </c>
       <c r="N40" s="2" t="s">
         <v>20</v>
@@ -20535,16 +20555,16 @@
     <hyperlink ref="C19" r:id="rId6"/>
     <hyperlink ref="E19" r:id="rId7"/>
     <hyperlink ref="C20" r:id="rId8"/>
-    <hyperlink ref="E20" r:id="rId9"/>
-    <hyperlink ref="C35" r:id="rId10"/>
-    <hyperlink ref="C36" r:id="rId11"/>
-    <hyperlink ref="E36" r:id="rId12"/>
-    <hyperlink ref="C38" r:id="rId13"/>
-    <hyperlink ref="E38" r:id="rId14"/>
-    <hyperlink ref="C39" r:id="rId15"/>
-    <hyperlink ref="E39" r:id="rId16"/>
-    <hyperlink ref="C40" r:id="rId17"/>
-    <hyperlink ref="E40" r:id="rId18"/>
+    <hyperlink ref="C35" r:id="rId9"/>
+    <hyperlink ref="C36" r:id="rId10"/>
+    <hyperlink ref="E36" r:id="rId11"/>
+    <hyperlink ref="C38" r:id="rId12"/>
+    <hyperlink ref="E38" r:id="rId13"/>
+    <hyperlink ref="C39" r:id="rId14"/>
+    <hyperlink ref="E39" r:id="rId15"/>
+    <hyperlink ref="C40" r:id="rId16"/>
+    <hyperlink ref="E40" r:id="rId17"/>
+    <hyperlink ref="E20" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add 17 09 + mt @SvyTo
</commit_message>
<xml_diff>
--- a/RPL_V2/xlsx/Матч Тура 24-25.xlsx
+++ b/RPL_V2/xlsx/Матч Тура 24-25.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4757" uniqueCount="1186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4764" uniqueCount="1190">
   <si>
     <t>type</t>
   </si>
@@ -3586,6 +3586,18 @@
   </si>
   <si>
     <t>17 июня 1923</t>
+  </si>
+  <si>
+    <t>31.07.24 Спартак 3:0 Динамо</t>
+  </si>
+  <si>
+    <t>Спартак 1:1 Динамо Махачкала</t>
+  </si>
+  <si>
+    <t>Динамо Москва 4:2 Ахмат</t>
+  </si>
+  <si>
+    <t>16 очков</t>
   </si>
 </sst>
 </file>
@@ -3655,7 +3667,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3669,6 +3681,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -18458,19 +18473,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="125" customWidth="1"/>
-    <col min="3" max="3" width="75" customWidth="1"/>
-    <col min="4" max="4" width="198" customWidth="1"/>
-    <col min="5" max="5" width="75" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" customWidth="1"/>
+    <col min="4" max="4" width="71.7109375" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26" customWidth="1"/>
+    <col min="7" max="7" width="30" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="24" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
@@ -18546,7 +18561,9 @@
       <c r="C2" s="2" t="s">
         <v>1051</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="E2" s="2" t="s">
         <v>1051</v>
       </c>
@@ -18597,7 +18614,9 @@
       <c r="C3" s="2" t="s">
         <v>1055</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>1068</v>
+      </c>
       <c r="E3" s="2" t="s">
         <v>1055</v>
       </c>
@@ -19637,7 +19656,7 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>729</v>
+        <v>1177</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>1177</v>
@@ -19686,14 +19705,16 @@
       <c r="C24" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D24" s="2"/>
+      <c r="D24" s="2" t="s">
+        <v>1187</v>
+      </c>
       <c r="E24" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="5" t="s">
         <v>1113</v>
       </c>
       <c r="H24" s="2" t="s">
@@ -19737,7 +19758,9 @@
       <c r="C25" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="2" t="s">
+        <v>1188</v>
+      </c>
       <c r="E25" s="2" t="s">
         <v>208</v>
       </c>
@@ -19788,7 +19811,9 @@
       <c r="C26" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>916</v>
+      </c>
       <c r="E26" s="2" t="s">
         <v>136</v>
       </c>
@@ -19839,7 +19864,9 @@
       <c r="C27" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="2"/>
+      <c r="D27" s="2" t="s">
+        <v>1189</v>
+      </c>
       <c r="E27" s="2" t="s">
         <v>132</v>
       </c>
@@ -20249,7 +20276,9 @@
       <c r="C35" s="3" t="s">
         <v>1086</v>
       </c>
-      <c r="D35" s="2"/>
+      <c r="D35" s="2" t="s">
+        <v>1186</v>
+      </c>
       <c r="E35" s="2" t="s">
         <v>136</v>
       </c>

</xml_diff>

<commit_message>
Add 23 09 + mt
</commit_message>
<xml_diff>
--- a/RPL_V2/xlsx/Матч Тура 24-25.xlsx
+++ b/RPL_V2/xlsx/Матч Тура 24-25.xlsx
@@ -3300,7 +3300,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q37"/>
+  <dimension ref="A1:Q39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5276,7 +5276,7 @@
       </c>
       <c r="D24" s="4" t="inlineStr">
         <is>
-          <t>2 гола в 6 матчах</t>
+          <t>5 голов в 9 матчах</t>
         </is>
       </c>
       <c r="E24" s="4" t="inlineStr">
@@ -5286,22 +5286,22 @@
       </c>
       <c r="F24" s="4" t="inlineStr">
         <is>
+          <t>kr_spertsjan</t>
+        </is>
+      </c>
+      <c r="G24" s="4" t="inlineStr">
+        <is>
+          <t>Эдуард Сперцян</t>
+        </is>
+      </c>
+      <c r="H24" s="4" t="inlineStr">
+        <is>
           <t>kr_mozes</t>
         </is>
       </c>
-      <c r="G24" s="4" t="inlineStr">
+      <c r="I24" s="4" t="inlineStr">
         <is>
           <t>Мозес</t>
-        </is>
-      </c>
-      <c r="H24" s="4" t="inlineStr">
-        <is>
-          <t>kr_spertsjan</t>
-        </is>
-      </c>
-      <c r="I24" s="4" t="inlineStr">
-        <is>
-          <t>Эдуард Сперцян</t>
         </is>
       </c>
       <c r="J24" s="4" t="inlineStr">
@@ -5359,7 +5359,11 @@
           <t>logo_zenit</t>
         </is>
       </c>
-      <c r="D25" s="4" t="n"/>
+      <c r="D25" s="4" t="inlineStr">
+        <is>
+          <t>7 голов в 6 играх</t>
+        </is>
+      </c>
       <c r="E25" s="4" t="inlineStr">
         <is>
           <t>zs_glushenkov</t>
@@ -5597,15 +5601,15 @@
           <t>Из какого клуба перешёл в Зенит забивной новичок Лусиано Гонду?</t>
         </is>
       </c>
-      <c r="C28" s="5" t="inlineStr">
-        <is>
-          <t>https://amaranth64.github.io/RPL_V2/matchday/images/zs_gondu.jpg</t>
+      <c r="C28" s="4" t="inlineStr">
+        <is>
+          <t>zs_gondu</t>
         </is>
       </c>
       <c r="D28" s="4" t="n"/>
-      <c r="E28" s="5" t="inlineStr">
-        <is>
-          <t>https://amaranth64.github.io/RPL_V2/matchday/images/zs_gondu.jpg</t>
+      <c r="E28" s="4" t="inlineStr">
+        <is>
+          <t>zs_gondu</t>
         </is>
       </c>
       <c r="F28" s="4" t="inlineStr">
@@ -6181,7 +6185,7 @@
       </c>
       <c r="B35" s="4" t="inlineStr">
         <is>
-          <t>Кто из этих футболистов Краснодара и Зенита за карьеру забил больше голов?</t>
+          <t>Кто из этих футболистов Краснодара и Зенита забил больше голов за карьеру?</t>
         </is>
       </c>
       <c r="C35" s="5" t="inlineStr">
@@ -6191,7 +6195,7 @@
       </c>
       <c r="D35" s="4" t="inlineStr">
         <is>
-          <t>Джон Кордоба - 129 мячей, Александр Соболев - 101</t>
+          <t>Джон Кордоба - 129 мячей, Александр Соболев - 101 мяч</t>
         </is>
       </c>
       <c r="E35" s="4" t="inlineStr">
@@ -6276,7 +6280,7 @@
       </c>
       <c r="D36" s="4" t="inlineStr">
         <is>
-          <t>Серебрянные медали Кубка Америки 2024</t>
+          <t>Серебрянная медаль Кубка Америки 2024</t>
         </is>
       </c>
       <c r="E36" s="4" t="inlineStr">
@@ -6425,6 +6429,168 @@
         </is>
       </c>
       <c r="Q37" s="4" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B38" s="4" t="inlineStr">
+        <is>
+          <t>Правда ли, что в составе Зенита присутствует Чемпион Европы по футболу?</t>
+        </is>
+      </c>
+      <c r="C38" s="4" t="inlineStr">
+        <is>
+          <t>logo_zenit</t>
+        </is>
+      </c>
+      <c r="D38" s="4" t="n"/>
+      <c r="E38" s="4" t="inlineStr">
+        <is>
+          <t>logo_zenit</t>
+        </is>
+      </c>
+      <c r="F38" s="4" t="inlineStr">
+        <is>
+          <t>no_pic</t>
+        </is>
+      </c>
+      <c r="G38" s="4" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="H38" s="4" t="inlineStr">
+        <is>
+          <t>no_pic</t>
+        </is>
+      </c>
+      <c r="I38" s="4" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="J38" s="4" t="inlineStr">
+        <is>
+          <t>no_pic</t>
+        </is>
+      </c>
+      <c r="K38" s="4" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="L38" s="4" t="inlineStr">
+        <is>
+          <t>no_pic</t>
+        </is>
+      </c>
+      <c r="M38" s="4" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="N38" s="4" t="inlineStr">
+        <is>
+          <t>no_pic</t>
+        </is>
+      </c>
+      <c r="O38" s="4" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="P38" s="4" t="inlineStr">
+        <is>
+          <t>no_pic</t>
+        </is>
+      </c>
+      <c r="Q38" s="4" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B39" s="4" t="inlineStr">
+        <is>
+          <t>Правда ли, что Страхинья Эракович был в заявке сборной Сербии на Чемпионате Мира по футболу 2022?</t>
+        </is>
+      </c>
+      <c r="C39" s="4" t="inlineStr">
+        <is>
+          <t>zs_erakovich</t>
+        </is>
+      </c>
+      <c r="D39" s="4" t="n"/>
+      <c r="E39" s="4" t="inlineStr">
+        <is>
+          <t>zs_erakovich</t>
+        </is>
+      </c>
+      <c r="F39" s="4" t="inlineStr">
+        <is>
+          <t>no_pic</t>
+        </is>
+      </c>
+      <c r="G39" s="4" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="H39" s="4" t="inlineStr">
+        <is>
+          <t>no_pic</t>
+        </is>
+      </c>
+      <c r="I39" s="4" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="J39" s="4" t="inlineStr">
+        <is>
+          <t>no_pic</t>
+        </is>
+      </c>
+      <c r="K39" s="4" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="L39" s="4" t="inlineStr">
+        <is>
+          <t>no_pic</t>
+        </is>
+      </c>
+      <c r="M39" s="4" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="N39" s="4" t="inlineStr">
+        <is>
+          <t>no_pic</t>
+        </is>
+      </c>
+      <c r="O39" s="4" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="P39" s="4" t="inlineStr">
+        <is>
+          <t>no_pic</t>
+        </is>
+      </c>
+      <c r="Q39" s="4" t="inlineStr">
         <is>
           <t>Нет</t>
         </is>
@@ -6434,14 +6600,12 @@
   <hyperlinks>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C21" r:id="rId1"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C22" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C28" r:id="rId3"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E28" r:id="rId4"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E29" r:id="rId5"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C30" r:id="rId6"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E30" r:id="rId7"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C35" r:id="rId8"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C37" r:id="rId9"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E37" r:id="rId10"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E29" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C30" r:id="rId4"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E30" r:id="rId5"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C35" r:id="rId6"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C37" r:id="rId7"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E37" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add 07 10 + mt
</commit_message>
<xml_diff>
--- a/RPL_V2/xlsx/Матч Тура 24-25.xlsx
+++ b/RPL_V2/xlsx/Матч Тура 24-25.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="mt_loko_krasnodar" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3190" uniqueCount="873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3404" uniqueCount="945">
   <si>
     <t>type</t>
   </si>
@@ -441,7 +441,7 @@
     <t>3 гола и 5 передач в 6 матчах</t>
   </si>
   <si>
-    <t>https://amaranth64.github.io/RPL_V2/matchday/images/loko_batrakov.jpg</t>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/https://amaranth64.github.io/RPL_V2/matchday/images/loko_batrakov.jpg</t>
   </si>
   <si>
     <t>На каком месте находится Краснодар после шести туров?</t>
@@ -546,13 +546,13 @@
     <t>Антон Митрюшкин</t>
   </si>
   <si>
-    <t>https://amaranth64.github.io/RPL_V2/matchday/mt_loko_krasnodar.jpg</t>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/https://amaranth64.github.io/RPL_V2/matchday/mt_loko_krasnodar.jpg</t>
   </si>
   <si>
     <t>Краснодар (2013 - 2017, 2018 - 2021), Локомотив (2017 - 2018)</t>
   </si>
   <si>
-    <t>https://amaranth64.github.io/RPL_V2/matchday/images/kr_ari.jpg</t>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/https://amaranth64.github.io/RPL_V2/matchday/images/kr_ari.jpg</t>
   </si>
   <si>
     <t>Даниил Уткин</t>
@@ -573,7 +573,7 @@
     <t>Краснодар (2019 - 2020), Локомотив (2014 - 2019)</t>
   </si>
   <si>
-    <t>https://amaranth64.github.io/RPL_V2/matchday/images/loko_manuel.jpg</t>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/https://amaranth64.github.io/RPL_V2/matchday/images/loko_manuel.jpg</t>
   </si>
   <si>
     <t>Мануэль Фернандеш</t>
@@ -738,7 +738,7 @@
     <t>Локомотив 2:2 Краснодар</t>
   </si>
   <si>
-    <t>https://amaranth64.github.io/RPL_V2/matchday/images/zs_sobolev.jpg</t>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/https://amaranth64.github.io/RPL_V2/matchday/images/zs_sobolev.jpg</t>
   </si>
   <si>
     <t>27-летний (07.03.1997) российский нападающий. Перешёл в Зенит в августе 2024 из Спартака</t>
@@ -762,7 +762,7 @@
     <t>Александр Ерохин</t>
   </si>
   <si>
-    <t>https://amaranth64.github.io/RPL_V2/matchday/images/zs_strahiny.jpg</t>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/https://amaranth64.github.io/RPL_V2/matchday/images/zs_strahiny.jpg</t>
   </si>
   <si>
     <t>23-летний (22.01.2001) сербский защитник. Перешёл в Зенит летом 2023 из Црвены Звезды</t>
@@ -783,7 +783,7 @@
     <t>Ильзат Ахметов</t>
   </si>
   <si>
-    <t>https://amaranth64.github.io/RPL_V2/matchday/images/zs_gondu.jpg</t>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/https://amaranth64.github.io/RPL_V2/matchday/images/zs_gondu.jpg</t>
   </si>
   <si>
     <t>23-летний (22.06.2001) аргентинский нападающий. Перешёл в Зенит в августе 2024 из Аргентинос Хуниорс</t>
@@ -849,7 +849,7 @@
     <t>Виктор Давила</t>
   </si>
   <si>
-    <t>https://amaranth64.github.io/RPL_V2/matchday/images/cska_musaev.jpg</t>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/https://amaranth64.github.io/RPL_V2/matchday/images/cska_musaev.jpg</t>
   </si>
   <si>
     <t>23-летний (29.07.2001) российский нападающий. Перешёл в ЦСКА зимой 2024 из Балтики</t>
@@ -864,7 +864,7 @@
     <t>Николай Баровский</t>
   </si>
   <si>
-    <t>https://amaranth64.github.io/RPL_V2/matchday/images/cska_faizulaev.jpg</t>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/https://amaranth64.github.io/RPL_V2/matchday/images/cska_faizulaev.jpg</t>
   </si>
   <si>
     <t>20-летний (03.10.2003) узбекский нападающий. Перешёл в ЦСКА летом 2023 из Пахтакора</t>
@@ -879,7 +879,7 @@
     <t>Кто из этих футболистов играл и за ЦСКА, и за Зенит?</t>
   </si>
   <si>
-    <t>https://amaranth64.github.io/RPL_V2/matchday/mt_cska_zenit.jpg</t>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/https://amaranth64.github.io/RPL_V2/matchday/mt_cska_zenit.jpg</t>
   </si>
   <si>
     <t>Саломон Рондон</t>
@@ -1239,7 +1239,7 @@
     <t>На первом месте по сыгранным матчам с капитанской повязкой за Зенит находится Александр Анюков (134 матча), на втором месте - Владислав Радимов (116 матчей), на третьем - Анатолий Тимощук (86 матчей)</t>
   </si>
   <si>
-    <t>https://amaranth64.github.io/RPL_V2/matchday/images/zs_anukov.jpg</t>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/https://amaranth64.github.io/RPL_V2/matchday/images/zs_anukov.jpg</t>
   </si>
   <si>
     <t>Александр Анюков</t>
@@ -1266,7 +1266,7 @@
     <t>Как зовут этого игрока Зенита - победителя Кубка УЕФА 2008?</t>
   </si>
   <si>
-    <t>https://amaranth64.github.io/RPL_V2/matchday/images/zs_faizulin_lg.webp</t>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/https://amaranth64.github.io/RPL_V2/matchday/images/zs_faizulin_lg.webp</t>
   </si>
   <si>
     <t>Виктор Файзулин</t>
@@ -1527,7 +1527,7 @@
     <t>Как зовут новичка Динамо Москва, пришедшего этим летом из Крузейро?</t>
   </si>
   <si>
-    <t>https://amaranth64.github.io/RPL_V2/matchday/images/dm_gomez.webp</t>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/https://amaranth64.github.io/RPL_V2/matchday/images/dm_gomez.webp</t>
   </si>
   <si>
     <t>Артур Гомес</t>
@@ -1551,7 +1551,7 @@
     <t>В какой клуб перешёл Антон Шунин после окончания контракта с Динамо Москва?</t>
   </si>
   <si>
-    <t>https://amaranth64.github.io/RPL_V2/matchday/images/dm_shunin.webp</t>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/https://amaranth64.github.io/RPL_V2/matchday/images/dm_shunin.webp</t>
   </si>
   <si>
     <t>Без клуба</t>
@@ -1566,7 +1566,7 @@
     <t>Кто из этих игроков играл и за Спартак, и за Динамо?</t>
   </si>
   <si>
-    <t>https://amaranth64.github.io/RPL_V2/matchday/images/mt_spartak_dinamo.jpg</t>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/https://amaranth64.github.io/RPL_V2/matchday/images/mt_spartak_dinamo.jpg</t>
   </si>
   <si>
     <t>sm_zobnin</t>
@@ -1866,7 +1866,7 @@
     <t>Кто этот знаменитый футболист, игрок Динамо в прошлом?</t>
   </si>
   <si>
-    <t>https://amaranth64.github.io/RPL_V2/matchday/images/dm_noboa.webp</t>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/https://amaranth64.github.io/RPL_V2/matchday/images/dm_noboa.webp</t>
   </si>
   <si>
     <t>Кристиан Нобоа</t>
@@ -2112,7 +2112,7 @@
     <t>Кто из этих игроков играл и за Краснодар, и за Зенит?</t>
   </si>
   <si>
-    <t>https://amaranth64.github.io/RPL_V2/matchday/images/mt_krasnodar_zenit.jpg</t>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/https://amaranth64.github.io/RPL_V2/matchday/images/mt_krasnodar_zenit.jpg</t>
   </si>
   <si>
     <t>Зенит (воспитанник - 2011), Краснодар(2013 - н.в.)</t>
@@ -2166,7 +2166,7 @@
     <t>Правда ли, что Игорь Смольников играл и за Зенит, и за Краснодар?</t>
   </si>
   <si>
-    <t>https://amaranth64.github.io/RPL_V2/matchday/images/zs_smolnikov.jpg</t>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/https://amaranth64.github.io/RPL_V2/matchday/images/zs_smolnikov.jpg</t>
   </si>
   <si>
     <t>Краснодар(2012 - 2013, 2020 - 2021), Зенит (2013 - 2020)</t>
@@ -2229,7 +2229,7 @@
     <t>Кто из этих игроков играл и за ЦСКА, и за Динамо?</t>
   </si>
   <si>
-    <t>https://amaranth64.github.io/RPL_V2/matchday/images/mt_dinamo_cska.jpg</t>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/https://amaranth64.github.io/RPL_V2/matchday/images/mt_dinamo_cska.jpg</t>
   </si>
   <si>
     <t>Ролан Гусев</t>
@@ -2391,7 +2391,7 @@
     <t>За какой из этих клубов не играл новичок ЦСКА Миралем Пьянич?</t>
   </si>
   <si>
-    <t>https://amaranth64.github.io/RPL_V2/matchday/images/cska_planic.jpg</t>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/https://amaranth64.github.io/RPL_V2/matchday/images/cska_planic.jpg</t>
   </si>
   <si>
     <t>Челси</t>
@@ -2451,7 +2451,7 @@
     <t>Как зовут форварда, который перешёл в ЦСКА из Сочи в сентябре?</t>
   </si>
   <si>
-    <t>https://amaranth64.github.io/RPL_V2/matchday/images/cska_saul.jpg</t>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/https://amaranth64.github.io/RPL_V2/matchday/images/cska_saul.jpg</t>
   </si>
   <si>
     <t>21-летний (18.10.2002) венесуэльский нападающий. Перешёл в ЦСКА осенью 2024 из Сочи</t>
@@ -2478,7 +2478,7 @@
     <t>26-летний (03.07.1998) бразильский нападающий. Перешёл в Динамо Москва осенью 2024 из Крузейро</t>
   </si>
   <si>
-    <t>https://amaranth64.github.io/RPL_V2/matchday/images/dm_maniche.jpg</t>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/https://amaranth64.github.io/RPL_V2/matchday/images/dm_maniche.jpg</t>
   </si>
   <si>
     <t>Играл в Динамо с 2005 по 2006</t>
@@ -2499,7 +2499,7 @@
     <t>Кто этот знаменитый футболист, игрок ЦСКА в прошлом?</t>
   </si>
   <si>
-    <t>https://amaranth64.github.io/RPL_V2/matchday/images/cska_karvalio.jpg</t>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/https://amaranth64.github.io/RPL_V2/matchday/images/cska_karvalio.jpg</t>
   </si>
   <si>
     <t>Играл в ЦСКА с 2004 по 2010 года</t>
@@ -2514,136 +2514,352 @@
     <t>Вагнер Лав</t>
   </si>
   <si>
+    <t>kr_djupin</t>
+  </si>
+  <si>
+    <t>Даниил Голиков</t>
+  </si>
+  <si>
+    <t>Дмитрий Пивоваров</t>
+  </si>
+  <si>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/sm_mangash.jpg</t>
+  </si>
+  <si>
+    <t>Рикарду Мангаш</t>
+  </si>
+  <si>
+    <t>27/10/2024 14:15</t>
+  </si>
+  <si>
+    <t>28/10/2024 18:30</t>
+  </si>
+  <si>
+    <t>Кого обыграл Спартак в прошлом туре?</t>
+  </si>
+  <si>
+    <t>Спартак 3:0 Ростов (Н. Умяров 29', Ш. Николсон 34', 45+4')</t>
+  </si>
+  <si>
+    <t>Краснодар 4:0 Химки (Д. Кордоба 41', 73'; Ж. Батчи 56', К. Кастано 89')</t>
+  </si>
+  <si>
+    <t>logog_fakel</t>
+  </si>
+  <si>
+    <t>Кто из этих игроков играл и за Краснодар, и за Спартак?</t>
+  </si>
+  <si>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/mt_spar_kras_quest.jpg</t>
+  </si>
+  <si>
+    <t>Спартак (2005 - 2009), Краснодар (2014 - 2017)</t>
+  </si>
+  <si>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/lg_bystrov.jpg</t>
+  </si>
+  <si>
+    <t>Владимир Быстров</t>
+  </si>
+  <si>
+    <t>Кто из этих игроков играл и за Спартак, и за Краснодар?</t>
+  </si>
+  <si>
+    <t>Спартак (2002 - 2007), Краснодар (2015 - 2017)</t>
+  </si>
+  <si>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/lg_torbinski.jpg</t>
+  </si>
+  <si>
+    <t>Дмитрий Торбинский</t>
+  </si>
+  <si>
+    <t>Дмитрий Комбаров</t>
+  </si>
+  <si>
+    <t>40-летний главный тренер Краснодара с середины сезона 2023/24</t>
+  </si>
+  <si>
+    <t>46-летний главный тренер Спартака с начала сезона 2024/25</t>
+  </si>
+  <si>
+    <t>Кто из текущих игроков Спартака дольше всех находится в клубе?</t>
+  </si>
+  <si>
+    <t>В команде с  1 июля 2016 года</t>
+  </si>
+  <si>
+    <t>sm_umjarov</t>
+  </si>
+  <si>
+    <t>Наиль Умяров</t>
+  </si>
+  <si>
+    <t>sm_duarte</t>
+  </si>
+  <si>
+    <t>sm_hlusevich</t>
+  </si>
+  <si>
+    <t>sm_maksimenko</t>
+  </si>
+  <si>
+    <t>Александр Максименко</t>
+  </si>
+  <si>
+    <t>sm_selihov</t>
+  </si>
+  <si>
+    <t>Александр Селихов</t>
+  </si>
+  <si>
+    <t>Кто из текущих игроков Краснодара дольше всех находится в клубе?</t>
+  </si>
+  <si>
+    <t>В команде с  2 января 2013 года/</t>
+  </si>
+  <si>
+    <t>kr_pantaleao</t>
+  </si>
+  <si>
+    <t>6 мячей в 11 матчах</t>
+  </si>
+  <si>
+    <t>6 мячей в 7 матчах</t>
+  </si>
+  <si>
+    <t>На каком месте находится Спартак после одиннадцати туров?</t>
+  </si>
+  <si>
+    <t>19 очков</t>
+  </si>
+  <si>
+    <t>На каком месте находится Краснодар после одиннадцати туров?</t>
+  </si>
+  <si>
+    <t>27 очков</t>
+  </si>
+  <si>
+    <t>Победой какой команды завершился последний матч между Спартаком и Краснодаром?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">РПЛ 23/24. Тур 28. Спартак Москва 1:0 Краснодар (Р. Зобнин 35') </t>
+  </si>
+  <si>
+    <t>Кто этот знаменитый футболист, игрок Спартака в прошлом?</t>
+  </si>
+  <si>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/sm_mazart.jpg</t>
+  </si>
+  <si>
+    <t>Сантос Моцарт выстуцпал за Спартак с 2005 по 2009 года. Сыграл 106 матчей и забил 13 голов</t>
+  </si>
+  <si>
+    <t>Моцарт</t>
+  </si>
+  <si>
+    <t>Пенише</t>
+  </si>
+  <si>
+    <t>Веллитон</t>
+  </si>
+  <si>
+    <t>Алекс</t>
+  </si>
+  <si>
+    <t>Ибсон</t>
+  </si>
+  <si>
+    <t>Рафаэл Кариока</t>
+  </si>
+  <si>
+    <t>Кто этот знаменитый футболист, игрок Краснодара в прошлом?</t>
+  </si>
+  <si>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/kr_matrynovich.jpg</t>
+  </si>
+  <si>
+    <t>Провёл 264 игры за Краснодар и забил 5 мячей</t>
+  </si>
+  <si>
+    <t>Александр Мартынович</t>
+  </si>
+  <si>
+    <t>Одил Ахмедов</t>
+  </si>
+  <si>
+    <t>Рикардо Лаборде</t>
+  </si>
+  <si>
+    <t>Какой из этих клубов чаще побеждал оппонента в официальных очных встречах?</t>
+  </si>
+  <si>
+    <t>19 побед Спартака и только 9 побед Краснодара</t>
+  </si>
+  <si>
+    <t>С каким счетом завершилась для Спартака встреча Ростовым в прошлом туре?</t>
+  </si>
+  <si>
+    <t>Спартак 3:0 Ростов</t>
+  </si>
+  <si>
+    <t>Спартак 3:1 Ростов</t>
+  </si>
+  <si>
+    <t>Спартак 3:2 Ростов</t>
+  </si>
+  <si>
+    <t>Спартак 2:0 Ростов</t>
+  </si>
+  <si>
+    <t>Спартак 1:1 Ростов</t>
+  </si>
+  <si>
+    <t>Спартак 0:1 Ростов</t>
+  </si>
+  <si>
+    <t>С каким счетом завершилась для Краснодара встреча с Химками в прошлом туре?</t>
+  </si>
+  <si>
+    <t>Краснодар 4:0 Химки</t>
+  </si>
+  <si>
+    <t>Краснодар 3:0 Химки</t>
+  </si>
+  <si>
+    <t>Краснодар 2:0 Химки</t>
+  </si>
+  <si>
+    <t>Краснодар 3:1 Химки</t>
+  </si>
+  <si>
+    <t>Краснодар 3:2 Химки</t>
+  </si>
+  <si>
+    <t>Краснодар 1:1 Химки</t>
+  </si>
+  <si>
+    <t>Когда состоялся первый матч между Спартаком и Краснодаром?</t>
+  </si>
+  <si>
+    <t>15.07.2009. Кубок России 1/16. Краснодар 1:2 Спартак</t>
+  </si>
+  <si>
+    <t>15 июля 2009 года</t>
+  </si>
+  <si>
+    <t>7 сентября 2011 года</t>
+  </si>
+  <si>
+    <t>11 ноября 2012 года</t>
+  </si>
+  <si>
+    <t>19 сентября 1987 года</t>
+  </si>
+  <si>
+    <t>21 апреля 1977 года</t>
+  </si>
+  <si>
+    <t>8 августа 1997 года</t>
+  </si>
+  <si>
+    <t>На каком стадионе пройдёт этот матч?</t>
+  </si>
+  <si>
+    <t>std_spartak</t>
+  </si>
+  <si>
+    <t>Лукойл Арена</t>
+  </si>
+  <si>
+    <t>В каком клубе сейчас играет бывший капитан Спартака Георгий Джикия?</t>
+  </si>
+  <si>
+    <t>sm_dzjikia</t>
+  </si>
+  <si>
+    <t>В какой клуб перешёл молодой российский игрок Леон Классен этим летом из Спартака?</t>
+  </si>
+  <si>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/sm_klassen.jpg</t>
+  </si>
+  <si>
+    <t>Ленгбю</t>
+  </si>
+  <si>
+    <t>Валюр</t>
+  </si>
+  <si>
+    <t>Хабнарфьордюр</t>
+  </si>
+  <si>
+    <t>Рейкьявик</t>
+  </si>
+  <si>
+    <t>Копенгаген</t>
+  </si>
+  <si>
+    <t>Мальме</t>
+  </si>
+  <si>
+    <t>Какой крупнейший счёт был в истории этого противостояния?</t>
+  </si>
+  <si>
+    <t>РПЛ 20/21. 21-й тур. Спартак 6:1 Краснодар (А. Соболев 1', 61'; К. Промес 8', Дж. Ларссон 63', 83'; Э. Понсе 75' - Ю. Газинский 56')</t>
+  </si>
+  <si>
+    <t>Спартак 6:1 Краснодар</t>
+  </si>
+  <si>
+    <t>Краснодар 4:0 Спартак</t>
+  </si>
+  <si>
+    <t>Спартак 2:7 Краснодар</t>
+  </si>
+  <si>
+    <t>Спартак 4:1 Краснодар</t>
+  </si>
+  <si>
+    <t>Спартак 5:2 Краснодар</t>
+  </si>
+  <si>
+    <t>Краснодар 5:0 Спартак</t>
+  </si>
+  <si>
+    <t>В каком клубе сейчас играет бывший игрок Спартака Джордан Ларсен?</t>
+  </si>
+  <si>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/sm_larsson.jpg</t>
+  </si>
+  <si>
+    <t>Зальцбург</t>
+  </si>
+  <si>
+    <t>Гамбург</t>
+  </si>
+  <si>
+    <t>ХИК</t>
+  </si>
+  <si>
+    <t>Спартак (2010 - 2013), Краснодар (2013 - 2021)</t>
+  </si>
+  <si>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/lg_ari.jpg</t>
+  </si>
+  <si>
+    <t>Андреас Гранквист</t>
+  </si>
+  <si>
+    <t>Стипе Плетикоса</t>
+  </si>
+  <si>
+    <t>Марсио Абреу</t>
+  </si>
+  <si>
     <t>На каком месте находится Динамо Москва после девяти туров?</t>
   </si>
   <si>
     <t>На каком месте находится ЦСКА после девяти туров?</t>
-  </si>
-  <si>
-    <t>Победой какой команды завершился последний матч между Спартаком и Краснодаром?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">РПЛ 23/24. Тур 28. Спартак Москва 1:0 Краснодар (Р. Зобнин 35') </t>
-  </si>
-  <si>
-    <t>Кто этот знаменитый футболист, игрок Спартака в прошлом?</t>
-  </si>
-  <si>
-    <t>Кто этот знаменитый футболист, игрок Краснодара в прошлом?</t>
-  </si>
-  <si>
-    <t>Кого обыграл Спартак в прошлом туре?</t>
-  </si>
-  <si>
-    <t>Кто из этих игроков играл и за Краснодар, и за Спартак?</t>
-  </si>
-  <si>
-    <t>Кто из этих игроков играл и за Спартак, и за Краснодар?</t>
-  </si>
-  <si>
-    <t>Кто из текущих игроков Спартака дольше всех находится в клубе?</t>
-  </si>
-  <si>
-    <t>Кто из текущих игроков Краснодара дольше всех находится в клубе?</t>
-  </si>
-  <si>
-    <t>На каком месте находится Спартак после девяти туров?</t>
-  </si>
-  <si>
-    <t>Когда состоялся первый матч между Спартаком и Краснодаром?</t>
-  </si>
-  <si>
-    <t>На каком стадионе пройдёт этот матч?</t>
-  </si>
-  <si>
-    <t>logog_fakel</t>
-  </si>
-  <si>
-    <t>С каким счетом завершилась для Краснодара встреча с Химками в прошлом туре?</t>
-  </si>
-  <si>
-    <t>С каким счетом завершилась для Спартака встреча Ростовым в прошлом туре?</t>
-  </si>
-  <si>
-    <t>mt_spar_kras_quest.jpg</t>
-  </si>
-  <si>
-    <t>40-летний главный тренер Краснодара с середины сезона 2023/24</t>
-  </si>
-  <si>
-    <t>46-летний главный тренер Спартака с начала сезона 2024/25</t>
-  </si>
-  <si>
-    <t>Вопрос про Абаскаля?</t>
-  </si>
-  <si>
-    <t>В команде с  1 июля 2016 года</t>
-  </si>
-  <si>
-    <t>kr_pantaleao</t>
-  </si>
-  <si>
-    <t>kr_djupin</t>
-  </si>
-  <si>
-    <t>В команде с  2 января 2013 года/</t>
-  </si>
-  <si>
-    <t>Рикарду Мангаш</t>
-  </si>
-  <si>
-    <t>В каком клубе сейчас играет бывший капитан Спартака Георгий Джикия?</t>
-  </si>
-  <si>
-    <t>В какой клуб перешёл молодой российский игрок Леон Классен этим летом из Спартака?</t>
-  </si>
-  <si>
-    <t>Ленгбю</t>
-  </si>
-  <si>
-    <t>Лукойл Арена</t>
-  </si>
-  <si>
-    <t>std_spartak</t>
-  </si>
-  <si>
-    <t>19 побед Спартака и только 9 побед Краснодара</t>
-  </si>
-  <si>
-    <t>Какой из этих клубов чаще побеждал оппонента в официальных очных встречах?</t>
-  </si>
-  <si>
-    <t>Какой крупнейший счёт был в истории этого противостояния?</t>
-  </si>
-  <si>
-    <t>Спартак 6:1 Краснодар</t>
-  </si>
-  <si>
-    <t>РПЛ 20/21. 21-й тур. Спартак 6:1 Краснодар (А. Соболев 1', 61'; К. Промес 8', Дж. Ларссон 63', 83'; Э. Понсе 75' - Ю. Газинский 56')</t>
-  </si>
-  <si>
-    <t>В каком клубе сейчас играет бывший игрок Спартака Джордан Ларсен?</t>
-  </si>
-  <si>
-    <t>Копенгаген</t>
-  </si>
-  <si>
-    <t>sm_larsson.jpg</t>
-  </si>
-  <si>
-    <t>sm_klassen.jpg</t>
-  </si>
-  <si>
-    <t>sm_dzjikia</t>
-  </si>
-  <si>
-    <t>sm_mangash.jpg</t>
-  </si>
-  <si>
-    <t>Даниил Голиков</t>
-  </si>
-  <si>
-    <t>Дмитрий Пивоваров</t>
   </si>
 </sst>
 </file>
@@ -2674,18 +2890,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -2719,7 +2929,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2729,12 +2939,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3041,16 +3245,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="78" customWidth="1"/>
-    <col min="3" max="3" width="68" customWidth="1"/>
-    <col min="5" max="5" width="71" customWidth="1"/>
+    <col min="3" max="3" width="120" customWidth="1"/>
+    <col min="5" max="5" width="123" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="25" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
@@ -4781,8 +4983,8 @@
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="85" customWidth="1"/>
-    <col min="3" max="3" width="73" customWidth="1"/>
-    <col min="5" max="5" width="73" customWidth="1"/>
+    <col min="3" max="3" width="125" customWidth="1"/>
+    <col min="5" max="5" width="125" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
@@ -6508,16 +6710,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="125" customWidth="1"/>
-    <col min="3" max="3" width="75" customWidth="1"/>
-    <col min="5" max="5" width="75" customWidth="1"/>
+    <col min="3" max="3" width="127" customWidth="1"/>
+    <col min="5" max="5" width="127" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="7" max="7" width="26" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
@@ -8637,16 +8837,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="104" customWidth="1"/>
-    <col min="3" max="3" width="76" customWidth="1"/>
-    <col min="5" max="5" width="73" customWidth="1"/>
+    <col min="3" max="3" width="128" customWidth="1"/>
+    <col min="5" max="5" width="125" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
@@ -10722,16 +10920,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="103" customWidth="1"/>
-    <col min="3" max="3" width="72" customWidth="1"/>
-    <col min="5" max="5" width="72" customWidth="1"/>
+    <col min="3" max="3" width="124" customWidth="1"/>
+    <col min="5" max="5" width="124" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="7" max="7" width="22" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
@@ -12629,28 +12825,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:Q4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="90.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" customWidth="1"/>
-    <col min="13" max="13" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11" customWidth="1"/>
-    <col min="15" max="15" width="20" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84" customWidth="1"/>
+    <col min="3" max="3" width="76" customWidth="1"/>
+    <col min="5" max="5" width="76" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="23" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="23" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
+    <col min="13" max="13" width="23" customWidth="1"/>
+    <col min="14" max="14" width="15" customWidth="1"/>
+    <col min="15" max="15" width="23" customWidth="1"/>
+    <col min="16" max="16" width="15" customWidth="1"/>
+    <col min="17" max="17" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -12707,296 +12903,320 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>635</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>636</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="2" t="s">
         <v>635</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="F2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>637</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="5" t="s">
+      <c r="H2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="5" t="s">
+      <c r="J2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="5" t="s">
+      <c r="L2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" s="5" t="s">
+      <c r="N2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="P2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q2" s="5" t="s">
+      <c r="P2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>638</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="2" t="s">
         <v>638</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="F3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>639</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="5" t="s">
+      <c r="H3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="5" t="s">
+      <c r="J3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M3" s="5" t="s">
+      <c r="L3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>640</v>
       </c>
-      <c r="N3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" s="5" t="s">
+      <c r="N3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="2" t="s">
         <v>641</v>
       </c>
-      <c r="P3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q3" s="5" t="s">
+      <c r="P3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>852</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="C4" s="2" t="s">
+        <v>829</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>681</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>852</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="E4" s="2" t="s">
+        <v>829</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="5" t="s">
+      <c r="H4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="J4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>871</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M4" s="5" t="s">
+      <c r="J4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>830</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>872</v>
-      </c>
-      <c r="P4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q4" s="5" t="s">
+      <c r="N4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q4" s="2" t="s">
         <v>639</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>870</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
-        <v>870</v>
-      </c>
-      <c r="F5" s="2"/>
+      <c r="C5" s="3" t="s">
+        <v>832</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>832</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="G5" s="2" t="s">
-        <v>854</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
+        <v>833</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="2">
         <v>1</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="5" t="s">
+      <c r="F6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="5" t="s">
+      <c r="H6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="J6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K6" s="5" t="s">
+      <c r="J6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="L6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M6" s="5" t="s">
+      <c r="L6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="N6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="O6" s="5" t="s">
+      <c r="N6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O6" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="P6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q6" s="5" t="s">
+      <c r="P6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q6" s="2" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="2">
         <v>1</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="5" t="s">
+      <c r="F7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="5" t="s">
+      <c r="H7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="J7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7" s="5" t="s">
+      <c r="J7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="L7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M7" s="5" t="s">
+      <c r="L7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="N7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="O7" s="5" t="s">
+      <c r="N7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O7" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="P7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q7" s="5" t="s">
+      <c r="P7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q7" s="2" t="s">
         <v>430</v>
       </c>
     </row>
@@ -13010,7 +13230,9 @@
       <c r="C8" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>834</v>
+      </c>
       <c r="E8" s="2" t="s">
         <v>377</v>
       </c>
@@ -13061,7 +13283,9 @@
       <c r="C9" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>835</v>
+      </c>
       <c r="E9" s="2" t="s">
         <v>545</v>
       </c>
@@ -13106,13 +13330,15 @@
       <c r="A10" s="2">
         <v>2</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>835</v>
+      <c r="B10" s="2" t="s">
+        <v>836</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>837</v>
+      </c>
       <c r="E10" s="2" t="s">
         <v>95</v>
       </c>
@@ -13157,13 +13383,15 @@
       <c r="A11" s="2">
         <v>2</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>118</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>838</v>
+      </c>
       <c r="E11" s="2" t="s">
         <v>114</v>
       </c>
@@ -13198,7 +13426,7 @@
         <v>104</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="Q11" s="2" t="s">
         <v>100</v>
@@ -13206,53 +13434,109 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>836</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>846</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
+        <v>840</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>841</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>843</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>844</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>837</v>
-      </c>
-      <c r="C13" s="2" t="s">
+        <v>845</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>841</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>846</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
+      <c r="E13" s="3" t="s">
+        <v>847</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>848</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>849</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -13265,7 +13549,7 @@
         <v>201</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>847</v>
+        <v>850</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>201</v>
@@ -13318,7 +13602,7 @@
         <v>462</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>848</v>
+        <v>851</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>462</v>
@@ -13365,13 +13649,13 @@
         <v>2</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>838</v>
+        <v>852</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>97</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>850</v>
+        <v>853</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>514</v>
@@ -13382,29 +13666,49 @@
       <c r="G16" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
+      <c r="H16" s="2" t="s">
+        <v>854</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>855</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>856</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>857</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>858</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>859</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>860</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>861</v>
+      </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>2</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>839</v>
+        <v>862</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>70</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>853</v>
+        <v>863</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>168</v>
@@ -13415,34 +13719,34 @@
       <c r="G17" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="H17" s="5" t="s">
-        <v>851</v>
-      </c>
-      <c r="I17" s="5" t="s">
+      <c r="H17" s="2" t="s">
+        <v>864</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="J17" s="2" t="s">
         <v>638</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="K17" s="2" t="s">
         <v>639</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="L17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M17" s="5" t="s">
+      <c r="M17" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="N17" s="5" t="s">
-        <v>852</v>
-      </c>
-      <c r="O17" s="5" t="s">
+      <c r="N17" s="2" t="s">
+        <v>829</v>
+      </c>
+      <c r="O17" s="2" t="s">
         <v>195</v>
       </c>
       <c r="P17" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="Q17" s="5" t="s">
+      <c r="Q17" s="2" t="s">
         <v>135</v>
       </c>
     </row>
@@ -13456,20 +13760,48 @@
       <c r="C18" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
+      <c r="D18" s="2" t="s">
+        <v>865</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
@@ -13481,85 +13813,171 @@
       <c r="C19" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>866</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>840</v>
+        <v>867</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>868</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
+      <c r="F20" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="O20" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>382</v>
+      </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>686</v>
+        <v>869</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>870</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2"/>
+      <c r="F21" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>6</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>831</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>846</v>
+        <v>871</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>841</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>832</v>
-      </c>
-      <c r="E22" s="2"/>
+        <v>872</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="F22" s="2" t="s">
         <v>20</v>
       </c>
@@ -13598,59 +14016,127 @@
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
+      <c r="A23" s="2">
+        <v>1</v>
+      </c>
       <c r="B23" s="2" t="s">
-        <v>833</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
+        <v>873</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>874</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>874</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>876</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>878</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>879</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>880</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>881</v>
+      </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
+      <c r="A24" s="2">
+        <v>1</v>
+      </c>
       <c r="B24" s="2" t="s">
-        <v>834</v>
-      </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
+        <v>882</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>883</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>884</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>883</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>885</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>886</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>887</v>
+      </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
+      <c r="A25" s="2">
+        <v>6</v>
+      </c>
       <c r="B25" s="2" t="s">
-        <v>861</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>846</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>860</v>
-      </c>
-      <c r="E25" s="5"/>
+        <v>888</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>841</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>889</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="F25" s="2" t="s">
         <v>20</v>
       </c>
@@ -13689,304 +14175,501 @@
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="4" t="s">
-        <v>845</v>
+      <c r="A26" s="2">
+        <v>1</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>890</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="5"/>
-      <c r="O26" s="5"/>
-      <c r="P26" s="5"/>
-      <c r="Q26" s="5"/>
+      <c r="D26" s="2" t="s">
+        <v>837</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>891</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>892</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>893</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>894</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>895</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>896</v>
+      </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="4" t="s">
-        <v>844</v>
+      <c r="A27" s="2">
+        <v>1</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>897</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
-      <c r="P27" s="5"/>
-      <c r="Q27" s="5"/>
+      <c r="D27" s="2" t="s">
+        <v>838</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>898</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>899</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>900</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>902</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>903</v>
+      </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
+      <c r="A28" s="2">
+        <v>1</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>904</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>841</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>905</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>841</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>906</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>907</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>908</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>909</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O28" s="2" t="s">
+        <v>910</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q28" s="2" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
         <v>6</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
+        <v>912</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>841</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>846</v>
-      </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5" t="s">
-        <v>859</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>858</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I28" s="5" t="s">
+      <c r="D29" s="2"/>
+      <c r="E29" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>914</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I29" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="J28" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K28" s="5" t="s">
+      <c r="J29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K29" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="L28" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M28" s="5" t="s">
+      <c r="L29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M29" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="N28" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O28" s="5" t="s">
+      <c r="N29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O29" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="P28" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q28" s="5" t="s">
+      <c r="P29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q29" s="2" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="2" t="s">
-        <v>842</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>846</v>
-      </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="5"/>
-    </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
+      <c r="A30" s="2">
+        <v>2</v>
+      </c>
       <c r="B30" s="2" t="s">
-        <v>849</v>
-      </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
-      <c r="O30" s="5"/>
-      <c r="P30" s="5"/>
-      <c r="Q30" s="5"/>
+        <v>915</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>916</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2" t="s">
+        <v>916</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="O30" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q30" s="2" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
+      <c r="A31" s="2">
+        <v>1</v>
+      </c>
       <c r="B31" s="2" t="s">
-        <v>855</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>869</v>
-      </c>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5" t="s">
-        <v>869</v>
+        <v>917</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>918</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="3" t="s">
+        <v>918</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>115</v>
+        <v>20</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>919</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>95</v>
+        <v>20</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>96</v>
+        <v>920</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>377</v>
+        <v>20</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>378</v>
+        <v>921</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>116</v>
+        <v>20</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>117</v>
+        <v>922</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>101</v>
+        <v>20</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>102</v>
+        <v>923</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>110</v>
+        <v>20</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>111</v>
+        <v>924</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
+      <c r="A32" s="2">
+        <v>1</v>
+      </c>
       <c r="B32" s="2" t="s">
-        <v>856</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>868</v>
-      </c>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5" t="s">
-        <v>868</v>
+        <v>925</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>841</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>926</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>841</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G32" s="5" t="s">
-        <v>857</v>
+      <c r="G32" s="2" t="s">
+        <v>927</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I32" s="5"/>
+      <c r="I32" s="2" t="s">
+        <v>928</v>
+      </c>
       <c r="J32" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K32" s="5"/>
+      <c r="K32" s="2" t="s">
+        <v>929</v>
+      </c>
       <c r="L32" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M32" s="5"/>
+      <c r="M32" s="2" t="s">
+        <v>930</v>
+      </c>
       <c r="N32" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O32" s="5"/>
+      <c r="O32" s="2" t="s">
+        <v>931</v>
+      </c>
       <c r="P32" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Q32" s="5"/>
-    </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q32" s="2" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>1</v>
+      </c>
       <c r="B33" s="2" t="s">
-        <v>862</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>846</v>
-      </c>
-      <c r="D33" t="s">
-        <v>864</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>846</v>
+        <v>933</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>934</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="3" t="s">
+        <v>934</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G33" s="5" t="s">
-        <v>863</v>
+      <c r="G33" s="2" t="s">
+        <v>923</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="I33" s="2" t="s">
+        <v>920</v>
+      </c>
       <c r="J33" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="K33" s="2" t="s">
+        <v>924</v>
+      </c>
       <c r="L33" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="M33" s="2" t="s">
+        <v>935</v>
+      </c>
       <c r="N33" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="O33" s="2" t="s">
+        <v>936</v>
+      </c>
       <c r="P33" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q33" s="2" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>1</v>
+      </c>
       <c r="B34" s="2" t="s">
-        <v>865</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>867</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>867</v>
+        <v>840</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>841</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>938</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>939</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G34" s="5" t="s">
-        <v>866</v>
+      <c r="G34" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="I34" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="J34" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="K34" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="L34" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="M34" s="2" t="s">
+        <v>940</v>
+      </c>
       <c r="N34" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="O34" s="2" t="s">
+        <v>941</v>
+      </c>
       <c r="P34" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="Q34" s="2" t="s">
+        <v>942</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1"/>
+    <hyperlink ref="E5" r:id="rId2"/>
+    <hyperlink ref="C12" r:id="rId3"/>
+    <hyperlink ref="E12" r:id="rId4"/>
+    <hyperlink ref="C13" r:id="rId5"/>
+    <hyperlink ref="E13" r:id="rId6"/>
+    <hyperlink ref="C22" r:id="rId7"/>
+    <hyperlink ref="C23" r:id="rId8"/>
+    <hyperlink ref="E23" r:id="rId9"/>
+    <hyperlink ref="C24" r:id="rId10"/>
+    <hyperlink ref="E24" r:id="rId11"/>
+    <hyperlink ref="C25" r:id="rId12"/>
+    <hyperlink ref="C28" r:id="rId13"/>
+    <hyperlink ref="E28" r:id="rId14"/>
+    <hyperlink ref="C29" r:id="rId15"/>
+    <hyperlink ref="C31" r:id="rId16"/>
+    <hyperlink ref="E31" r:id="rId17"/>
+    <hyperlink ref="C32" r:id="rId18"/>
+    <hyperlink ref="E32" r:id="rId19"/>
+    <hyperlink ref="C33" r:id="rId20"/>
+    <hyperlink ref="E33" r:id="rId21"/>
+    <hyperlink ref="C34" r:id="rId22"/>
+    <hyperlink ref="E34" r:id="rId23"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -13994,18 +14677,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="75" customWidth="1"/>
+    <col min="2" max="2" width="89" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="17" width="11" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="17" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -14480,7 +15162,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>829</v>
+        <v>943</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -14503,7 +15185,7 @@
         <v>2</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>830</v>
+        <v>944</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -14526,11 +15208,11 @@
         <v>6</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>831</v>
+        <v>871</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>832</v>
+        <v>872</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
@@ -14571,44 +15253,188 @@
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>2</v>
+      </c>
       <c r="B23" s="2" t="s">
-        <v>833</v>
-      </c>
+        <v>873</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>2</v>
+      </c>
       <c r="B24" s="2" t="s">
-        <v>834</v>
-      </c>
+        <v>882</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>2</v>
+      </c>
       <c r="B25" s="2" t="s">
         <v>779</v>
       </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>2</v>
+      </c>
       <c r="B26" s="2" t="s">
         <v>547</v>
       </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>2</v>
+      </c>
       <c r="B27" s="2" t="s">
         <v>547</v>
       </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>2</v>
+      </c>
       <c r="B28" s="2" t="s">
         <v>526</v>
       </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>2</v>
+      </c>
       <c r="B29" s="2" t="s">
-        <v>842</v>
-      </c>
+        <v>912</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>2</v>
+      </c>
       <c r="B30" s="2" t="s">
-        <v>862</v>
-      </c>
+        <v>925</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add 08 10 + mt
</commit_message>
<xml_diff>
--- a/RPL_V2/xlsx/Матч Тура 24-25.xlsx
+++ b/RPL_V2/xlsx/Матч Тура 24-25.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3404" uniqueCount="945">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3404" uniqueCount="944">
   <si>
     <t>type</t>
   </si>
@@ -2544,9 +2544,6 @@
     <t>Краснодар 4:0 Химки (Д. Кордоба 41', 73'; Ж. Батчи 56', К. Кастано 89')</t>
   </si>
   <si>
-    <t>logog_fakel</t>
-  </si>
-  <si>
     <t>Кто из этих игроков играл и за Краснодар, и за Спартак?</t>
   </si>
   <si>
@@ -2697,9 +2694,6 @@
     <t>19 побед Спартака и только 9 побед Краснодара</t>
   </si>
   <si>
-    <t>С каким счетом завершилась для Спартака встреча Ростовым в прошлом туре?</t>
-  </si>
-  <si>
     <t>Спартак 3:0 Ростов</t>
   </si>
   <si>
@@ -2860,6 +2854,9 @@
   </si>
   <si>
     <t>На каком месте находится ЦСКА после девяти туров?</t>
+  </si>
+  <si>
+    <t>С каким счетом завершилась для Спартака встреча Ростовом в прошлом туре?</t>
   </si>
 </sst>
 </file>
@@ -12825,7 +12822,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13424,7 +13423,7 @@
         <v>104</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>839</v>
+        <v>99</v>
       </c>
       <c r="Q11" s="2" t="s">
         <v>100</v>
@@ -13435,22 +13434,22 @@
         <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>839</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>840</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>841</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="3" t="s">
         <v>842</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>843</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>844</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>20</v>
@@ -13488,22 +13487,22 @@
         <v>1</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>844</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>840</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>845</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>841</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="3" t="s">
         <v>846</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="F13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>847</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>848</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>20</v>
@@ -13533,7 +13532,7 @@
         <v>20</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -13547,7 +13546,7 @@
         <v>201</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>201</v>
@@ -13600,7 +13599,7 @@
         <v>462</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>462</v>
@@ -13647,13 +13646,13 @@
         <v>2</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>97</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>514</v>
@@ -13665,34 +13664,34 @@
         <v>515</v>
       </c>
       <c r="H16" s="2" t="s">
+        <v>853</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>854</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="J16" s="2" t="s">
         <v>855</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>856</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>430</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>422</v>
       </c>
       <c r="N16" s="2" t="s">
+        <v>857</v>
+      </c>
+      <c r="O16" s="2" t="s">
         <v>858</v>
       </c>
-      <c r="O16" s="2" t="s">
+      <c r="P16" s="2" t="s">
         <v>859</v>
       </c>
-      <c r="P16" s="2" t="s">
+      <c r="Q16" s="2" t="s">
         <v>860</v>
-      </c>
-      <c r="Q16" s="2" t="s">
-        <v>861</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -13700,13 +13699,13 @@
         <v>2</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>70</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>168</v>
@@ -13718,7 +13717,7 @@
         <v>169</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>32</v>
@@ -13759,7 +13758,7 @@
         <v>97</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>569</v>
@@ -13812,7 +13811,7 @@
         <v>70</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>131</v>
@@ -13859,13 +13858,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>866</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>867</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>868</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>97</v>
@@ -13912,13 +13911,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>868</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>869</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>870</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>70</v>
@@ -13965,13 +13964,13 @@
         <v>6</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>870</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>840</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>871</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>841</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>872</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>97</v>
@@ -14018,52 +14017,52 @@
         <v>1</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>872</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>873</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>874</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="3" t="s">
+        <v>873</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>875</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>874</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G23" s="2" t="s">
+      <c r="H23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" s="2" t="s">
         <v>876</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I23" s="2" t="s">
+      <c r="J23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K23" s="2" t="s">
         <v>877</v>
       </c>
-      <c r="J23" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K23" s="2" t="s">
+      <c r="L23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M23" s="2" t="s">
         <v>878</v>
       </c>
-      <c r="L23" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M23" s="2" t="s">
+      <c r="N23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O23" s="2" t="s">
         <v>879</v>
       </c>
-      <c r="N23" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O23" s="2" t="s">
+      <c r="P23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q23" s="2" t="s">
         <v>880</v>
-      </c>
-      <c r="P23" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q23" s="2" t="s">
-        <v>881</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -14071,22 +14070,22 @@
         <v>1</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>881</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>882</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="2" t="s">
         <v>883</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="3" t="s">
+        <v>882</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>884</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>883</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>885</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>20</v>
@@ -14110,13 +14109,13 @@
         <v>20</v>
       </c>
       <c r="O24" s="2" t="s">
+        <v>885</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q24" s="2" t="s">
         <v>886</v>
-      </c>
-      <c r="P24" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q24" s="2" t="s">
-        <v>887</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -14124,13 +14123,13 @@
         <v>6</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>887</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>840</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>888</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>841</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>889</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>97</v>
@@ -14177,7 +14176,7 @@
         <v>1</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>890</v>
+        <v>943</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>97</v>
@@ -14192,37 +14191,37 @@
         <v>20</v>
       </c>
       <c r="G26" s="2" t="s">
+        <v>889</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>890</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K26" s="2" t="s">
         <v>891</v>
       </c>
-      <c r="H26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I26" s="2" t="s">
+      <c r="L26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M26" s="2" t="s">
         <v>892</v>
       </c>
-      <c r="J26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K26" s="2" t="s">
+      <c r="N26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O26" s="2" t="s">
         <v>893</v>
       </c>
-      <c r="L26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M26" s="2" t="s">
+      <c r="P26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q26" s="2" t="s">
         <v>894</v>
-      </c>
-      <c r="N26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O26" s="2" t="s">
-        <v>895</v>
-      </c>
-      <c r="P26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q26" s="2" t="s">
-        <v>896</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -14230,7 +14229,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>70</v>
@@ -14245,37 +14244,37 @@
         <v>20</v>
       </c>
       <c r="G27" s="2" t="s">
+        <v>896</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>897</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K27" s="2" t="s">
         <v>898</v>
       </c>
-      <c r="H27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I27" s="2" t="s">
+      <c r="L27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M27" s="2" t="s">
         <v>899</v>
       </c>
-      <c r="J27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K27" s="2" t="s">
+      <c r="N27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O27" s="2" t="s">
         <v>900</v>
       </c>
-      <c r="L27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M27" s="2" t="s">
+      <c r="P27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q27" s="2" t="s">
         <v>901</v>
-      </c>
-      <c r="N27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O27" s="2" t="s">
-        <v>902</v>
-      </c>
-      <c r="P27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q27" s="2" t="s">
-        <v>903</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -14283,52 +14282,52 @@
         <v>1</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>902</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>840</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>903</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>840</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>904</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>841</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="H28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I28" s="2" t="s">
         <v>905</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>841</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28" s="2" t="s">
+      <c r="J28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K28" s="2" t="s">
         <v>906</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I28" s="2" t="s">
+      <c r="L28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M28" s="2" t="s">
         <v>907</v>
       </c>
-      <c r="J28" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K28" s="2" t="s">
+      <c r="N28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O28" s="2" t="s">
         <v>908</v>
       </c>
-      <c r="L28" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M28" s="2" t="s">
+      <c r="P28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q28" s="2" t="s">
         <v>909</v>
-      </c>
-      <c r="N28" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O28" s="2" t="s">
-        <v>910</v>
-      </c>
-      <c r="P28" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q28" s="2" t="s">
-        <v>911</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -14336,20 +14335,20 @@
         <v>6</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>20</v>
@@ -14387,14 +14386,14 @@
         <v>2</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="3" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>114</v>
@@ -14438,50 +14437,50 @@
         <v>1</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="3" t="s">
+        <v>916</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>917</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I31" s="2" t="s">
         <v>918</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G31" s="2" t="s">
+      <c r="J31" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K31" s="2" t="s">
         <v>919</v>
       </c>
-      <c r="H31" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I31" s="2" t="s">
+      <c r="L31" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M31" s="2" t="s">
         <v>920</v>
       </c>
-      <c r="J31" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K31" s="2" t="s">
+      <c r="N31" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O31" s="2" t="s">
         <v>921</v>
       </c>
-      <c r="L31" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M31" s="2" t="s">
+      <c r="P31" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q31" s="2" t="s">
         <v>922</v>
-      </c>
-      <c r="N31" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O31" s="2" t="s">
-        <v>923</v>
-      </c>
-      <c r="P31" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q31" s="2" t="s">
-        <v>924</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -14489,52 +14488,52 @@
         <v>1</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>923</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>840</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>924</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>840</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>925</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>841</v>
-      </c>
-      <c r="D32" s="2" t="s">
+      <c r="H32" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I32" s="2" t="s">
         <v>926</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>841</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G32" s="2" t="s">
+      <c r="J32" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K32" s="2" t="s">
         <v>927</v>
       </c>
-      <c r="H32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I32" s="2" t="s">
+      <c r="L32" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M32" s="2" t="s">
         <v>928</v>
       </c>
-      <c r="J32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K32" s="2" t="s">
+      <c r="N32" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O32" s="2" t="s">
         <v>929</v>
       </c>
-      <c r="L32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M32" s="2" t="s">
+      <c r="P32" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q32" s="2" t="s">
         <v>930</v>
-      </c>
-      <c r="N32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O32" s="2" t="s">
-        <v>931</v>
-      </c>
-      <c r="P32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q32" s="2" t="s">
-        <v>932</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -14542,50 +14541,50 @@
         <v>1</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="3" t="s">
+        <v>932</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>921</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>918</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>922</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>933</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O33" s="2" t="s">
         <v>934</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>923</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>920</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>924</v>
-      </c>
-      <c r="L33" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M33" s="2" t="s">
+      <c r="P33" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q33" s="2" t="s">
         <v>935</v>
-      </c>
-      <c r="N33" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O33" s="2" t="s">
-        <v>936</v>
-      </c>
-      <c r="P33" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q33" s="2" t="s">
-        <v>937</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
@@ -14593,16 +14592,16 @@
         <v>1</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>839</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>840</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>841</v>
-      </c>
       <c r="D34" s="2" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>20</v>
@@ -14626,19 +14625,19 @@
         <v>20</v>
       </c>
       <c r="M34" s="2" t="s">
+        <v>938</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>939</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q34" s="2" t="s">
         <v>940</v>
-      </c>
-      <c r="N34" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O34" s="2" t="s">
-        <v>941</v>
-      </c>
-      <c r="P34" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q34" s="2" t="s">
-        <v>942</v>
       </c>
     </row>
   </sheetData>
@@ -14658,16 +14657,16 @@
     <hyperlink ref="C28" r:id="rId13"/>
     <hyperlink ref="E28" r:id="rId14"/>
     <hyperlink ref="C29" r:id="rId15"/>
-    <hyperlink ref="C30" r:id="rId16"/>
-    <hyperlink ref="E30" r:id="rId17"/>
-    <hyperlink ref="C31" r:id="rId18"/>
-    <hyperlink ref="E31" r:id="rId19"/>
-    <hyperlink ref="C32" r:id="rId20"/>
-    <hyperlink ref="E32" r:id="rId21"/>
-    <hyperlink ref="C33" r:id="rId22"/>
-    <hyperlink ref="E33" r:id="rId23"/>
-    <hyperlink ref="C34" r:id="rId24"/>
-    <hyperlink ref="E34" r:id="rId25"/>
+    <hyperlink ref="C31" r:id="rId16"/>
+    <hyperlink ref="E31" r:id="rId17"/>
+    <hyperlink ref="C32" r:id="rId18"/>
+    <hyperlink ref="E32" r:id="rId19"/>
+    <hyperlink ref="C33" r:id="rId20"/>
+    <hyperlink ref="E33" r:id="rId21"/>
+    <hyperlink ref="C34" r:id="rId22"/>
+    <hyperlink ref="E34" r:id="rId23"/>
+    <hyperlink ref="E30" r:id="rId24"/>
+    <hyperlink ref="C30" r:id="rId25"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15162,7 +15161,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -15185,7 +15184,7 @@
         <v>2</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -15208,11 +15207,11 @@
         <v>6</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
@@ -15257,7 +15256,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -15280,7 +15279,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -15395,7 +15394,7 @@
         <v>2</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -15418,7 +15417,7 @@
         <v>2</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>

</xml_diff>

<commit_message>
Add 20 11 + mt
</commit_message>
<xml_diff>
--- a/RPL_V2/xlsx/Матч Тура 24-25.xlsx
+++ b/RPL_V2/xlsx/Матч Тура 24-25.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6063" uniqueCount="1449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6063" uniqueCount="1450">
   <si>
     <t>type</t>
   </si>
@@ -4376,6 +4376,9 @@
   </si>
   <si>
     <t>lm_samoshnikov</t>
+  </si>
+  <si>
+    <t>8 голов в 15 матчах</t>
   </si>
 </sst>
 </file>
@@ -7684,7 +7687,7 @@
   <dimension ref="A1:Q37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7692,6 +7695,7 @@
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="77" customWidth="1"/>
     <col min="3" max="3" width="84" customWidth="1"/>
+    <col min="4" max="4" width="37.5703125" customWidth="1"/>
     <col min="5" max="5" width="84" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
@@ -8615,7 +8619,7 @@
         <v>97</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>1055</v>
+        <v>1449</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>569</v>
@@ -8668,7 +8672,7 @@
         <v>108</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>967</v>
+        <v>1321</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>944</v>

</xml_diff>

<commit_message>
Add mt 26 11
</commit_message>
<xml_diff>
--- a/RPL_V2/xlsx/Матч Тура 24-25.xlsx
+++ b/RPL_V2/xlsx/Матч Тура 24-25.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="7" activeTab="12"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="7" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="mt_loko_krasnodar" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6606" uniqueCount="1467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6574" uniqueCount="1484">
   <si>
     <t>type</t>
   </si>
@@ -4233,6 +4233,9 @@
     <t>https://amaranth64.github.io/RPL_V2/matchday/images/sm_samedov.jpg</t>
   </si>
   <si>
+    <t>8 голов в 15 матчах</t>
+  </si>
+  <si>
     <t>На каком месте находится Спартак после пятнадцати туров?</t>
   </si>
   <si>
@@ -4347,15 +4350,15 @@
     <t>Ивелин Попов</t>
   </si>
   <si>
+    <t>Гилерме</t>
+  </si>
+  <si>
     <t>https://amaranth64.github.io/RPL_V2/matchday/images/sm_ze_luis.jpg</t>
   </si>
   <si>
     <t>Зе Луиш</t>
   </si>
   <si>
-    <t>Гилерме</t>
-  </si>
-  <si>
     <t>Лоренцо Мельгарехо</t>
   </si>
   <si>
@@ -4380,64 +4383,115 @@
     <t>lm_samoshnikov</t>
   </si>
   <si>
-    <t>8 голов в 15 матчах</t>
-  </si>
-  <si>
-    <t>Краснодар 2:1 Факел (А. Батраков 29', 90+2' - Е. Марков 84')</t>
+    <t>Спартак 5:2 Акрон (М. Угальде 10', 21', 34, 73'; Э. Барко 80' - С. Пиняев 55', Ж. Ньямси 63')</t>
+  </si>
+  <si>
+    <t>Химки 2:2 Краснодар (А. Руденко 84', Д. Вера (пен) 90+4' - Ж. Бахти 84', Ю. Газинский 86')</t>
+  </si>
+  <si>
+    <t>https://amaranth64.github.io/RPL_V2/matchday/images/mt_spartak_krasnodar_quest.jpg</t>
+  </si>
+  <si>
+    <t>12 голов в 16 матчах</t>
+  </si>
+  <si>
+    <t>8 мячей в 12 матчах</t>
+  </si>
+  <si>
+    <t>На каком месте находится Спартак после шестнадцати туров?</t>
+  </si>
+  <si>
+    <t>31 очко</t>
+  </si>
+  <si>
+    <t>На каком месте находится Краснодар после шестнадцати туров?</t>
+  </si>
+  <si>
+    <t>38 очков</t>
   </si>
   <si>
     <t>Как завершился последний матч между Спартаком и Краснодаром?</t>
   </si>
   <si>
-    <t>РПЛ 24/25. Тур 10. Краснодар 3:1 Спартак (И. Самошников 7', 36', Д. Воробьев 58' - Э. Барко(пен) 16')</t>
-  </si>
-  <si>
-    <t>Краснодар 3:1 Спартак</t>
-  </si>
-  <si>
-    <t>Краснодар 1:1 Спартак</t>
-  </si>
-  <si>
-    <t>Краснодар 0:1 Спартак</t>
-  </si>
-  <si>
-    <t>Краснодар 1:3 Спартак</t>
-  </si>
-  <si>
-    <t>Краснодар 0:0 Спартак</t>
-  </si>
-  <si>
-    <t>Краснодар 2:1 Спартак</t>
+    <t>РПЛ 24/25. Тур 12. Спартак 0:3 Краснодар (К. Ленини 8', Виктор Са 45', Х. Медина (аг) 90+6')</t>
+  </si>
+  <si>
+    <t>Спартак 0:3 Краснодар</t>
+  </si>
+  <si>
+    <t>Спартак 1:1 Краснодар</t>
+  </si>
+  <si>
+    <t>Спартак 0:1 Краснодар</t>
+  </si>
+  <si>
+    <t>Спартак 1:3 Краснодар</t>
+  </si>
+  <si>
+    <t>Спартак 0:0 Краснодар</t>
+  </si>
+  <si>
+    <t>Спартак 2:1 Краснодар</t>
+  </si>
+  <si>
+    <t>С каким счетом завершилась для Спартака встреча с Локомотивом в прошлом туре?</t>
+  </si>
+  <si>
+    <t>Спартак 5:2 Локомотив</t>
+  </si>
+  <si>
+    <t>Спартак 5:0 Локомотив</t>
+  </si>
+  <si>
+    <t>Спартак 1:0 Локомотив</t>
+  </si>
+  <si>
+    <t>Спартак 3:2 Локомотив</t>
+  </si>
+  <si>
+    <t>Спартак 0:2 Локомотив</t>
+  </si>
+  <si>
+    <t>Спартак 0:0 Локомотив</t>
+  </si>
+  <si>
+    <t>Химки 2:2 Краснодар</t>
+  </si>
+  <si>
+    <t>Химки 2:1 Краснодар</t>
+  </si>
+  <si>
+    <t>Химки 1:2 Краснодар</t>
+  </si>
+  <si>
+    <t>Химки 1:1 Краснодар</t>
+  </si>
+  <si>
+    <t>Химки 0:4 Краснодар</t>
+  </si>
+  <si>
+    <t>Химки 0:3 Краснодар</t>
   </si>
   <si>
     <t>На каком стадионе пройдёт матч между Краснодаром и Спартаком?</t>
   </si>
   <si>
-    <t>Кто из этих футболистов никогда не играл за Краснодар?</t>
-  </si>
-  <si>
-    <t>https://amaranth64.github.io/RPL_V2/matchday/images/mt_spartak_krasnodar_quest.jpg</t>
-  </si>
-  <si>
-    <t>На каком месте находится Спартак после шестнадцати туров?</t>
-  </si>
-  <si>
-    <t>На каком месте находится Краснодар после шестнадцати туров?</t>
-  </si>
-  <si>
-    <t>Химки 2:1 Краснодар</t>
-  </si>
-  <si>
-    <t>С каким счетом завершилась для Спартака встреча с Локомотивом в прошлом туре?</t>
-  </si>
-  <si>
     <t>std_krasnodar</t>
+  </si>
+  <si>
+    <t>07.12.2024  14:00</t>
+  </si>
+  <si>
+    <t>08.12.2024  19:30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4462,18 +4516,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -4518,10 +4566,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4829,9 +4877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B32"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7751,16 +7797,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="77" customWidth="1"/>
     <col min="3" max="3" width="84" customWidth="1"/>
-    <col min="4" max="4" width="37.5703125" customWidth="1"/>
     <col min="5" max="5" width="84" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
@@ -8684,7 +8727,7 @@
         <v>97</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>1449</v>
+        <v>1400</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>569</v>
@@ -8784,13 +8827,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>97</v>
@@ -8837,7 +8880,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>20</v>
@@ -8890,13 +8933,13 @@
         <v>1</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>1396</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>1396</v>
@@ -8905,37 +8948,37 @@
         <v>20</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="N22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="P22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -8946,11 +8989,11 @@
         <v>872</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="3" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>20</v>
@@ -8968,7 +9011,7 @@
         <v>20</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>20</v>
@@ -8986,7 +9029,7 @@
         <v>20</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -8997,23 +9040,23 @@
         <v>982</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="3" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>20</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>20</v>
@@ -9025,19 +9068,19 @@
         <v>20</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="N24" s="2" t="s">
         <v>20</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="P24" s="2" t="s">
         <v>20</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -9045,7 +9088,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>97</v>
@@ -9060,37 +9103,37 @@
         <v>20</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>20</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>20</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="N25" s="2" t="s">
         <v>20</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="P25" s="2" t="s">
         <v>20</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -9098,7 +9141,7 @@
         <v>1</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>108</v>
@@ -9113,37 +9156,37 @@
         <v>20</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>20</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>20</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="N26" s="2" t="s">
         <v>20</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="P26" s="2" t="s">
         <v>20</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -9151,7 +9194,7 @@
         <v>6</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>1396</v>
@@ -9202,14 +9245,14 @@
         <v>1</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>1396</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="3" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>20</v>
@@ -9221,13 +9264,13 @@
         <v>20</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>20</v>
@@ -9245,7 +9288,7 @@
         <v>20</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -9253,32 +9296,32 @@
         <v>1</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>1396</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="3" t="s">
-        <v>1438</v>
+        <v>1440</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G29" s="2" t="s">
+        <v>1441</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I29" s="2" t="s">
         <v>1439</v>
       </c>
-      <c r="H29" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>1440</v>
-      </c>
       <c r="J29" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>20</v>
@@ -9290,7 +9333,7 @@
         <v>20</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="P29" s="2" t="s">
         <v>20</v>
@@ -9304,14 +9347,14 @@
         <v>1</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>97</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="3" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>20</v>
@@ -9335,7 +9378,7 @@
         <v>20</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="N30" s="2" t="s">
         <v>20</v>
@@ -9355,14 +9398,14 @@
         <v>1</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>108</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="3" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>20</v>
@@ -9380,7 +9423,7 @@
         <v>20</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="L31" s="2" t="s">
         <v>20</v>
@@ -9406,7 +9449,7 @@
         <v>5</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>20</v>
@@ -9422,7 +9465,7 @@
         <v>172</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>53</v>
@@ -9738,31 +9781,31 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="78.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.85546875" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.28515625" customWidth="1"/>
-    <col min="16" max="16" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="2" max="2" width="79" customWidth="1"/>
+    <col min="3" max="3" width="84" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="84" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="23" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="23" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
+    <col min="13" max="13" width="23" customWidth="1"/>
+    <col min="14" max="14" width="15" customWidth="1"/>
+    <col min="15" max="15" width="23" customWidth="1"/>
+    <col min="16" max="16" width="13" customWidth="1"/>
+    <col min="17" max="17" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -10146,8 +10189,8 @@
       <c r="C8" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="4">
-        <v>45633.583333333336</v>
+      <c r="D8" s="5" t="s">
+        <v>1482</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>377</v>
@@ -10199,8 +10242,8 @@
       <c r="C9" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="4">
-        <v>45634.8125</v>
+      <c r="D9" s="5" t="s">
+        <v>1483</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>108</v>
@@ -10252,8 +10295,8 @@
       <c r="C10" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>1392</v>
+      <c r="D10" s="2" t="s">
+        <v>1450</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>108</v>
@@ -10305,8 +10348,8 @@
       <c r="C11" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>1450</v>
+      <c r="D11" s="2" t="s">
+        <v>1451</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>114</v>
@@ -10353,84 +10396,103 @@
         <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>839</v>
+        <v>844</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>1461</v>
+        <v>1452</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="E12" s="3" t="s">
+        <v>1399</v>
+      </c>
       <c r="F12" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>1265</v>
+        <v>78</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>20</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>515</v>
+        <v>177</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>73</v>
+        <v>302</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>20</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>1124</v>
+        <v>631</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O12" s="2"/>
+      <c r="O12" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="P12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Q12" s="2"/>
+      <c r="Q12" s="2" t="s">
+        <v>1442</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>1</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>844</v>
+        <v>839</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>1461</v>
-      </c>
-      <c r="D13" s="2"/>
+        <v>840</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>841</v>
+      </c>
       <c r="E13" s="3" t="s">
-        <v>1399</v>
+        <v>842</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>78</v>
+        <v>843</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="2"/>
+      <c r="I13" s="2" t="s">
+        <v>184</v>
+      </c>
       <c r="J13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K13" s="2"/>
+      <c r="K13" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="L13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M13" s="2"/>
+      <c r="M13" s="2" t="s">
+        <v>633</v>
+      </c>
       <c r="N13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O13" s="2"/>
+      <c r="O13" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="P13" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -10438,52 +10500,52 @@
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>839</v>
+        <v>844</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>840</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>841</v>
+        <v>845</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>842</v>
+        <v>846</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>843</v>
+        <v>847</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>20</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>64</v>
+        <v>291</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>20</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>633</v>
+        <v>515</v>
       </c>
       <c r="N14" s="2" t="s">
         <v>20</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>73</v>
+        <v>631</v>
       </c>
       <c r="P14" s="2" t="s">
         <v>20</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>302</v>
+        <v>848</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -10491,52 +10553,52 @@
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>844</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>840</v>
+        <v>200</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>201</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>845</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>846</v>
+        <v>849</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>201</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>847</v>
+        <v>203</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>20</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>177</v>
+        <v>204</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>291</v>
+        <v>205</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>20</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>515</v>
+        <v>206</v>
       </c>
       <c r="N15" s="2" t="s">
         <v>20</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>631</v>
+        <v>207</v>
       </c>
       <c r="P15" s="2" t="s">
         <v>20</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>848</v>
+        <v>208</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -10544,105 +10606,105 @@
         <v>1</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>200</v>
+        <v>461</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>201</v>
+        <v>462</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>201</v>
+        <v>462</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>203</v>
+        <v>463</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>20</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>204</v>
+        <v>464</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>205</v>
+        <v>465</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>20</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>206</v>
+        <v>466</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>20</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>207</v>
+        <v>326</v>
       </c>
       <c r="P16" s="2" t="s">
         <v>20</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>208</v>
+        <v>467</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>461</v>
+        <v>851</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>462</v>
+        <v>97</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>850</v>
+        <v>852</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>462</v>
+        <v>514</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>20</v>
+        <v>514</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>463</v>
+        <v>515</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>20</v>
+        <v>853</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>464</v>
+        <v>854</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>20</v>
+        <v>855</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>465</v>
+        <v>430</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>20</v>
+        <v>856</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>466</v>
+        <v>422</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>20</v>
+        <v>857</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>326</v>
+        <v>858</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>20</v>
+        <v>859</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>467</v>
+        <v>860</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -10650,52 +10712,52 @@
         <v>2</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>851</v>
+        <v>861</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>852</v>
+        <v>862</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>514</v>
+        <v>168</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>514</v>
+        <v>168</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>515</v>
+        <v>169</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>853</v>
+        <v>863</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>854</v>
+        <v>32</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>855</v>
+        <v>638</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>430</v>
+        <v>639</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>856</v>
+        <v>34</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>422</v>
+        <v>36</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>857</v>
+        <v>829</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>858</v>
+        <v>195</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>859</v>
+        <v>72</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>860</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -10703,52 +10765,52 @@
         <v>2</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>861</v>
+        <v>620</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>70</v>
+        <v>97</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>862</v>
+        <v>1453</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>168</v>
+        <v>569</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>168</v>
+        <v>569</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>169</v>
+        <v>421</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>863</v>
+        <v>432</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>32</v>
+        <v>434</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>638</v>
+        <v>621</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>639</v>
+        <v>435</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>34</v>
+        <v>514</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>36</v>
+        <v>515</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>829</v>
+        <v>623</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>195</v>
+        <v>624</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>72</v>
+        <v>436</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>135</v>
+        <v>428</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -10756,105 +10818,105 @@
         <v>2</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>620</v>
+        <v>129</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>1449</v>
+        <v>70</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>1454</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>569</v>
+        <v>131</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>569</v>
+        <v>131</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>421</v>
+        <v>132</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>432</v>
+        <v>27</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>434</v>
+        <v>29</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>621</v>
+        <v>34</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>435</v>
+        <v>36</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>514</v>
+        <v>133</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>515</v>
+        <v>134</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>623</v>
+        <v>72</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>624</v>
+        <v>135</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>436</v>
+        <v>42</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>428</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>129</v>
+        <v>1455</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>1212</v>
+        <v>20</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>1456</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>131</v>
+        <v>97</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>29</v>
+        <v>141</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>36</v>
+        <v>144</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>133</v>
+        <v>91</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>42</v>
+        <v>381</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>25</v>
+        <v>382</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -10862,105 +10924,105 @@
         <v>4</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>1462</v>
+        <v>1457</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>1401</v>
+      <c r="D22" s="2" t="s">
+        <v>1458</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="F22" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="N22" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="O22" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="N22" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="P22" s="2" t="s">
-        <v>381</v>
+        <v>89</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>382</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>1459</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>1452</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>1460</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>1452</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>1461</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>1462</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K23" s="2" t="s">
         <v>1463</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>1364</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>141</v>
-      </c>
       <c r="L23" s="2" t="s">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>143</v>
+        <v>1464</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>144</v>
+        <v>1465</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>145</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -10968,52 +11030,52 @@
         <v>1</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>1451</v>
+        <v>872</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>1461</v>
+        <v>873</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>1452</v>
+        <v>874</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>1461</v>
+        <v>873</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>1453</v>
+        <v>875</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>20</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>1454</v>
+        <v>876</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>1455</v>
+        <v>877</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>20</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>1456</v>
+        <v>878</v>
       </c>
       <c r="N24" s="2" t="s">
         <v>20</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>1457</v>
+        <v>879</v>
       </c>
       <c r="P24" s="2" t="s">
         <v>20</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>1458</v>
+        <v>880</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -11021,52 +11083,52 @@
         <v>1</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>872</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>873</v>
+        <v>1467</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>874</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>873</v>
+        <v>1450</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>875</v>
+        <v>1468</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>20</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>876</v>
+        <v>1469</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>877</v>
+        <v>1470</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>20</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>878</v>
+        <v>1471</v>
       </c>
       <c r="N25" s="2" t="s">
         <v>20</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>879</v>
+        <v>1472</v>
       </c>
       <c r="P25" s="2" t="s">
         <v>20</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>880</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -11074,87 +11136,103 @@
         <v>1</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>881</v>
-      </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="3"/>
+        <v>896</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>1451</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="F26" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G26" s="2"/>
+      <c r="G26" s="2" t="s">
+        <v>1474</v>
+      </c>
       <c r="H26" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I26" s="2"/>
+      <c r="I26" s="2" t="s">
+        <v>1475</v>
+      </c>
       <c r="J26" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K26" s="2"/>
+      <c r="K26" s="2" t="s">
+        <v>1476</v>
+      </c>
       <c r="L26" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M26" s="2"/>
+      <c r="M26" s="2" t="s">
+        <v>1477</v>
+      </c>
       <c r="N26" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O26" s="2"/>
+      <c r="O26" s="2" t="s">
+        <v>1478</v>
+      </c>
       <c r="P26" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Q26" s="2"/>
+      <c r="Q26" s="2" t="s">
+        <v>1479</v>
+      </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>1465</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>1392</v>
-      </c>
+        <v>1480</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>1452</v>
+      </c>
+      <c r="D27" s="2"/>
       <c r="E27" s="2" t="s">
-        <v>97</v>
+        <v>1481</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>1421</v>
+        <v>347</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>20</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>1422</v>
+        <v>1106</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>1423</v>
+        <v>1106</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>20</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>1424</v>
+        <v>1106</v>
       </c>
       <c r="N27" s="2" t="s">
         <v>20</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>1425</v>
+        <v>1106</v>
       </c>
       <c r="P27" s="2" t="s">
         <v>20</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>1426</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -11162,309 +11240,132 @@
         <v>1</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>896</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>70</v>
+        <v>924</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>840</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>1450</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>70</v>
+        <v>925</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>840</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G28" s="2"/>
+      <c r="G28" s="2" t="s">
+        <v>926</v>
+      </c>
       <c r="H28" s="2" t="s">
         <v>20</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>1464</v>
+        <v>927</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>1464</v>
+        <v>928</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>20</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>1464</v>
+        <v>929</v>
       </c>
       <c r="N28" s="2" t="s">
         <v>20</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>1464</v>
+        <v>930</v>
       </c>
       <c r="P28" s="2" t="s">
         <v>20</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>1464</v>
+        <v>931</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>1459</v>
+        <v>903</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>1461</v>
-      </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2" t="s">
-        <v>1466</v>
+        <v>840</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>904</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>840</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>347</v>
+        <v>905</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>20</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>1106</v>
+        <v>906</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>1106</v>
+        <v>907</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>20</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>1106</v>
+        <v>908</v>
       </c>
       <c r="N29" s="2" t="s">
         <v>20</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>1106</v>
+        <v>909</v>
       </c>
       <c r="P29" s="2" t="s">
         <v>20</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>1106</v>
+        <v>910</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>1</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>1442</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>1128</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M30" s="2" t="s">
-        <v>1444</v>
-      </c>
-      <c r="N30" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O30" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="P30" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q30" s="2" t="s">
-        <v>1124</v>
-      </c>
+      <c r="D30" s="4"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>1</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>1460</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>1</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>924</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>840</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>925</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>840</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>926</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>927</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>928</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M32" s="2" t="s">
-        <v>929</v>
-      </c>
-      <c r="N32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O32" s="2" t="s">
-        <v>930</v>
-      </c>
-      <c r="P32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q32" s="2" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <v>1</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>903</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>840</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>904</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>840</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>905</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>906</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>907</v>
-      </c>
-      <c r="L33" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M33" s="2" t="s">
-        <v>908</v>
-      </c>
-      <c r="N33" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O33" s="2" t="s">
-        <v>909</v>
-      </c>
-      <c r="P33" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q33" s="2" t="s">
-        <v>910</v>
-      </c>
+      <c r="D31" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C12" r:id="rId1" display="https://amaranth64.github.io/RPL_V2/matchday/images/mt_spartak_lokomotiv_quest.jpg"/>
-    <hyperlink ref="C13" r:id="rId2" display="https://amaranth64.github.io/RPL_V2/matchday/images/mt_spartak_lokomotiv_quest.jpg"/>
-    <hyperlink ref="E13" r:id="rId3"/>
-    <hyperlink ref="C14" r:id="rId4"/>
-    <hyperlink ref="E14" r:id="rId5"/>
-    <hyperlink ref="C15" r:id="rId6"/>
-    <hyperlink ref="E15" r:id="rId7"/>
-    <hyperlink ref="C32" r:id="rId8"/>
-    <hyperlink ref="E32" r:id="rId9"/>
-    <hyperlink ref="C25" r:id="rId10"/>
-    <hyperlink ref="E25" r:id="rId11"/>
-    <hyperlink ref="C5" r:id="rId12"/>
-    <hyperlink ref="E5" r:id="rId13"/>
-    <hyperlink ref="C33" r:id="rId14"/>
-    <hyperlink ref="E33" r:id="rId15"/>
+    <hyperlink ref="C5" r:id="rId1"/>
+    <hyperlink ref="E5" r:id="rId2"/>
+    <hyperlink ref="C12" r:id="rId3"/>
+    <hyperlink ref="E12" r:id="rId4"/>
+    <hyperlink ref="C13" r:id="rId5"/>
+    <hyperlink ref="E13" r:id="rId6"/>
+    <hyperlink ref="C14" r:id="rId7"/>
+    <hyperlink ref="E14" r:id="rId8"/>
+    <hyperlink ref="C23" r:id="rId9"/>
+    <hyperlink ref="E23" r:id="rId10"/>
+    <hyperlink ref="C24" r:id="rId11"/>
+    <hyperlink ref="E24" r:id="rId12"/>
+    <hyperlink ref="C27" r:id="rId13"/>
+    <hyperlink ref="C28" r:id="rId14"/>
+    <hyperlink ref="E28" r:id="rId15"/>
+    <hyperlink ref="C29" r:id="rId16"/>
+    <hyperlink ref="E29" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11474,14 +11375,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="80" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="2" max="2" width="78" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="17" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -11539,83 +11442,233 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>69</v>
       </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -11624,6 +11677,21 @@
       <c r="B12" s="2" t="s">
         <v>93</v>
       </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -11632,6 +11700,21 @@
       <c r="B13" s="2" t="s">
         <v>107</v>
       </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -11640,6 +11723,21 @@
       <c r="B14" s="2" t="s">
         <v>118</v>
       </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
@@ -11648,6 +11746,21 @@
       <c r="B15" s="2" t="s">
         <v>127</v>
       </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -11656,134 +11769,389 @@
       <c r="B16" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>2</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>2</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>229</v>
       </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19642,9 +20010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -21494,9 +21860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -25296,9 +25660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView topLeftCell="F10" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21:Q21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>